<commit_message>
Ex Bảng cửu chương _ Basic
</commit_message>
<xml_diff>
--- a/1.nen-tang-lap-trinh-java/5.vong-lap.xlsx
+++ b/1.nen-tang-lap-trinh-java/5.vong-lap.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\java\1.nen-tang-lap-trinh-java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250358DF-445C-4273-B041-AB6842AE5D07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A77765C4-8ECA-46C3-928E-0287E1CF528A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30225" yWindow="1050" windowWidth="26070" windowHeight="13830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30225" yWindow="1050" windowWidth="26070" windowHeight="13830" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vòng lặp" sheetId="1" r:id="rId1"/>
+    <sheet name="Ex Bảng cửu chương _ Basic" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="49">
   <si>
     <t>java_training</t>
     <phoneticPr fontId="1"/>
@@ -705,6 +706,75 @@
       </rPr>
       <t>c thi</t>
     </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>edit</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>int number = 9;</t>
+  </si>
+  <si>
+    <t>System.out.println("=============FOR=============");</t>
+  </si>
+  <si>
+    <t>System.out.println("=============WHILE=============");</t>
+  </si>
+  <si>
+    <t>System.out.printf("%d x %d = %d%n", number, j, number*j);</t>
+  </si>
+  <si>
+    <t>System.out.println("=============DO WHILE=============");</t>
+  </si>
+  <si>
+    <t>System.out.printf("%d x %d = %d%n", number, k, number*k);</t>
+  </si>
+  <si>
+    <t>}while(k &lt;= 10);</t>
+  </si>
+  <si>
+    <t>// 001 LOOP</t>
+  </si>
+  <si>
+    <t>public static void main001(String[] args) {</t>
+  </si>
+  <si>
+    <t>java_training\src\ph1_basic\p05_loop.java</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>System.out.printf("%d x %d = %d%n", number, i, number*i);</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>%n: Xu</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>ố</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ng dòng</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://docs.oracle.com/javase/tutorial/java/data/numberformat.html</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -862,7 +932,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -873,9 +943,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1096,6 +1170,196 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>255428</xdr:colOff>
+      <xdr:row>133</xdr:row>
+      <xdr:rowOff>189605</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="図 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07160C74-6610-1104-4F88-BC500D7515BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="742950" y="15887700"/>
+          <a:ext cx="13971428" cy="7161905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>137</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>65776</xdr:colOff>
+      <xdr:row>167</xdr:row>
+      <xdr:rowOff>189628</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="図 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3B07EF7-9C20-D06D-4A49-5711E2B385BE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="23850600"/>
+          <a:ext cx="7193651" cy="6971428"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>227188</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>69021</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="図 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C95AB7B8-0512-AAF1-814C-0D92310B37C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="3267075"/>
+          <a:ext cx="11295238" cy="6628571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="直線矢印コネクタ 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57614526-92EC-2004-87E2-35041747499C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1047750" y="5381625"/>
+          <a:ext cx="6924675" cy="7467600"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1366,8 +1630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:N70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="O44" sqref="O44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -1419,7 +1683,7 @@
     </row>
     <row r="9" spans="2:11">
       <c r="B9" s="4"/>
-      <c r="E9" s="10" t="s">
+      <c r="E9" t="s">
         <v>6</v>
       </c>
       <c r="G9" s="5"/>
@@ -1466,152 +1730,72 @@
     </row>
     <row r="16" spans="2:11">
       <c r="B16" s="4"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
       <c r="K16" s="5"/>
     </row>
     <row r="17" spans="2:13">
       <c r="B17" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
       <c r="K17" s="5"/>
     </row>
     <row r="18" spans="2:13">
       <c r="B18" s="4"/>
-      <c r="C18" s="11" t="s">
+      <c r="C18" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
       <c r="K18" s="5"/>
     </row>
     <row r="19" spans="2:13">
       <c r="B19" s="4"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11" t="s">
+      <c r="D19" t="s">
         <v>14</v>
       </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
       <c r="K19" s="5"/>
     </row>
     <row r="20" spans="2:13">
       <c r="B20" s="4"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11" t="s">
+      <c r="D20" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
       <c r="K20" s="5"/>
     </row>
     <row r="21" spans="2:13">
       <c r="B21" s="4"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11" t="s">
+      <c r="E21" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
       <c r="K21" s="5"/>
     </row>
     <row r="22" spans="2:13">
       <c r="B22" s="4"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11" t="s">
+      <c r="D22" t="s">
         <v>17</v>
       </c>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
       <c r="K22" s="5"/>
     </row>
     <row r="23" spans="2:13">
       <c r="B23" s="4"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
       <c r="K23" s="5"/>
     </row>
     <row r="24" spans="2:13">
       <c r="B24" s="4"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11" t="s">
+      <c r="D24" t="s">
         <v>18</v>
       </c>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
       <c r="K24" s="5"/>
     </row>
     <row r="25" spans="2:13">
       <c r="B25" s="4"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11" t="s">
+      <c r="D25" t="s">
         <v>19</v>
       </c>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
       <c r="K25" s="5"/>
     </row>
     <row r="26" spans="2:13">
       <c r="B26" s="4"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11" t="s">
+      <c r="D26" t="s">
         <v>20</v>
       </c>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
       <c r="K26" s="5"/>
       <c r="L26" t="s">
         <v>7</v>
@@ -1622,98 +1806,48 @@
     </row>
     <row r="27" spans="2:13">
       <c r="B27" s="4"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11" t="s">
+      <c r="E27" t="s">
         <v>21</v>
       </c>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
       <c r="K27" s="5"/>
     </row>
     <row r="28" spans="2:13">
       <c r="B28" s="4"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11" t="s">
+      <c r="E28" t="s">
         <v>22</v>
       </c>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
       <c r="K28" s="5"/>
     </row>
     <row r="29" spans="2:13">
       <c r="B29" s="4"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11" t="s">
+      <c r="D29" t="s">
         <v>17</v>
       </c>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11"/>
       <c r="K29" s="5"/>
     </row>
     <row r="30" spans="2:13">
       <c r="B30" s="4"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
       <c r="K30" s="5"/>
     </row>
     <row r="31" spans="2:13">
       <c r="B31" s="4"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11" t="s">
+      <c r="D31" t="s">
         <v>23</v>
       </c>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11"/>
       <c r="K31" s="5"/>
     </row>
     <row r="32" spans="2:13">
       <c r="B32" s="4"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11" t="s">
+      <c r="D32" t="s">
         <v>24</v>
       </c>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
       <c r="K32" s="5"/>
     </row>
     <row r="33" spans="2:14">
       <c r="B33" s="4"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11" t="s">
+      <c r="D33" t="s">
         <v>25</v>
       </c>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="11"/>
       <c r="K33" s="5"/>
       <c r="L33" t="s">
         <v>7</v>
@@ -1725,16 +1859,9 @@
     </row>
     <row r="34" spans="2:14">
       <c r="B34" s="4"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11" t="s">
+      <c r="E34" t="s">
         <v>26</v>
       </c>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
       <c r="K34" s="5"/>
       <c r="M34" s="6"/>
       <c r="N34" s="6" t="s">
@@ -1743,18 +1870,12 @@
     </row>
     <row r="35" spans="2:14">
       <c r="B35" s="4"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11" t="s">
+      <c r="E35" t="s">
         <v>27</v>
       </c>
-      <c r="F35" s="11" t="s">
+      <c r="F35" t="s">
         <v>28</v>
       </c>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="11"/>
       <c r="K35" s="5"/>
       <c r="M35" s="6"/>
       <c r="N35" s="6" t="s">
@@ -1763,16 +1884,9 @@
     </row>
     <row r="36" spans="2:14">
       <c r="B36" s="4"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11" t="s">
+      <c r="D36" t="s">
         <v>29</v>
       </c>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="11"/>
       <c r="K36" s="5"/>
       <c r="L36" t="s">
         <v>7</v>
@@ -1783,30 +1897,15 @@
     </row>
     <row r="37" spans="2:14">
       <c r="B37" s="4"/>
-      <c r="C37" s="11" t="s">
+      <c r="C37" t="s">
         <v>17</v>
       </c>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="11"/>
       <c r="K37" s="5"/>
     </row>
     <row r="38" spans="2:14">
       <c r="B38" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="11"/>
       <c r="K38" s="5"/>
     </row>
     <row r="39" spans="2:14">
@@ -1822,7 +1921,7 @@
       <c r="K39" s="9"/>
     </row>
     <row r="42" spans="2:14">
-      <c r="B42" s="12" t="s">
+      <c r="B42" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C42" s="2"/>
@@ -1837,326 +1936,110 @@
     </row>
     <row r="43" spans="2:14">
       <c r="B43" s="4"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="11"/>
-      <c r="H43" s="11"/>
-      <c r="I43" s="11"/>
-      <c r="J43" s="11"/>
       <c r="K43" s="5"/>
     </row>
     <row r="44" spans="2:14">
       <c r="B44" s="4"/>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
-      <c r="I44" s="11"/>
-      <c r="J44" s="11"/>
       <c r="K44" s="5"/>
     </row>
     <row r="45" spans="2:14">
       <c r="B45" s="4"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
-      <c r="I45" s="11"/>
-      <c r="J45" s="11"/>
       <c r="K45" s="5"/>
     </row>
     <row r="46" spans="2:14">
       <c r="B46" s="4"/>
-      <c r="C46" s="11"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11"/>
-      <c r="I46" s="11"/>
-      <c r="J46" s="11"/>
       <c r="K46" s="5"/>
     </row>
     <row r="47" spans="2:14">
       <c r="B47" s="4"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
-      <c r="I47" s="11"/>
-      <c r="J47" s="11"/>
       <c r="K47" s="5"/>
     </row>
     <row r="48" spans="2:14">
       <c r="B48" s="4"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
-      <c r="I48" s="11"/>
-      <c r="J48" s="11"/>
       <c r="K48" s="5"/>
     </row>
     <row r="49" spans="2:11">
       <c r="B49" s="4"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11"/>
-      <c r="F49" s="11"/>
-      <c r="G49" s="11"/>
-      <c r="H49" s="11"/>
-      <c r="I49" s="11"/>
-      <c r="J49" s="11"/>
       <c r="K49" s="5"/>
     </row>
     <row r="50" spans="2:11">
       <c r="B50" s="4"/>
-      <c r="C50" s="11"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
-      <c r="G50" s="11"/>
-      <c r="H50" s="11"/>
-      <c r="I50" s="11"/>
-      <c r="J50" s="11"/>
       <c r="K50" s="5"/>
     </row>
     <row r="51" spans="2:11">
       <c r="B51" s="4"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11"/>
-      <c r="I51" s="11"/>
-      <c r="J51" s="11"/>
       <c r="K51" s="5"/>
     </row>
     <row r="52" spans="2:11">
       <c r="B52" s="4"/>
-      <c r="C52" s="11"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="11"/>
-      <c r="F52" s="11"/>
-      <c r="G52" s="11"/>
-      <c r="H52" s="11"/>
-      <c r="I52" s="11"/>
-      <c r="J52" s="11"/>
       <c r="K52" s="5"/>
     </row>
     <row r="53" spans="2:11">
       <c r="B53" s="4"/>
-      <c r="C53" s="11"/>
-      <c r="D53" s="11"/>
-      <c r="E53" s="11"/>
-      <c r="F53" s="11"/>
-      <c r="G53" s="11"/>
-      <c r="H53" s="11"/>
-      <c r="I53" s="11"/>
-      <c r="J53" s="11"/>
       <c r="K53" s="5"/>
     </row>
     <row r="54" spans="2:11">
       <c r="B54" s="4"/>
-      <c r="C54" s="11"/>
-      <c r="D54" s="11"/>
-      <c r="E54" s="11"/>
-      <c r="F54" s="11"/>
-      <c r="G54" s="11"/>
-      <c r="H54" s="11"/>
-      <c r="I54" s="11"/>
-      <c r="J54" s="11"/>
       <c r="K54" s="5"/>
     </row>
     <row r="55" spans="2:11">
       <c r="B55" s="4"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
-      <c r="E55" s="11"/>
-      <c r="F55" s="11"/>
-      <c r="G55" s="11"/>
-      <c r="H55" s="11"/>
-      <c r="I55" s="11"/>
-      <c r="J55" s="11"/>
       <c r="K55" s="5"/>
     </row>
     <row r="56" spans="2:11">
       <c r="B56" s="4"/>
-      <c r="C56" s="11"/>
-      <c r="D56" s="11"/>
-      <c r="E56" s="11"/>
-      <c r="F56" s="11"/>
-      <c r="G56" s="11"/>
-      <c r="H56" s="11"/>
-      <c r="I56" s="11"/>
-      <c r="J56" s="11"/>
       <c r="K56" s="5"/>
     </row>
     <row r="57" spans="2:11">
       <c r="B57" s="4"/>
-      <c r="C57" s="11"/>
-      <c r="D57" s="11"/>
-      <c r="E57" s="11"/>
-      <c r="F57" s="11"/>
-      <c r="G57" s="11"/>
-      <c r="H57" s="11"/>
-      <c r="I57" s="11"/>
-      <c r="J57" s="11"/>
       <c r="K57" s="5"/>
     </row>
     <row r="58" spans="2:11">
       <c r="B58" s="4"/>
-      <c r="C58" s="11"/>
-      <c r="D58" s="11"/>
-      <c r="E58" s="11"/>
-      <c r="F58" s="11"/>
-      <c r="G58" s="11"/>
-      <c r="H58" s="11"/>
-      <c r="I58" s="11"/>
-      <c r="J58" s="11"/>
       <c r="K58" s="5"/>
     </row>
     <row r="59" spans="2:11">
       <c r="B59" s="4"/>
-      <c r="C59" s="11"/>
-      <c r="D59" s="11"/>
-      <c r="E59" s="11"/>
-      <c r="F59" s="11"/>
-      <c r="G59" s="11"/>
-      <c r="H59" s="11"/>
-      <c r="I59" s="11"/>
-      <c r="J59" s="11"/>
       <c r="K59" s="5"/>
     </row>
     <row r="60" spans="2:11">
       <c r="B60" s="4"/>
-      <c r="C60" s="11"/>
-      <c r="D60" s="11"/>
-      <c r="E60" s="11"/>
-      <c r="F60" s="11"/>
-      <c r="G60" s="11"/>
-      <c r="H60" s="11"/>
-      <c r="I60" s="11"/>
-      <c r="J60" s="11"/>
       <c r="K60" s="5"/>
     </row>
     <row r="61" spans="2:11">
       <c r="B61" s="4"/>
-      <c r="C61" s="11"/>
-      <c r="D61" s="11"/>
-      <c r="E61" s="11"/>
-      <c r="F61" s="11"/>
-      <c r="G61" s="11"/>
-      <c r="H61" s="11"/>
-      <c r="I61" s="11"/>
-      <c r="J61" s="11"/>
       <c r="K61" s="5"/>
     </row>
     <row r="62" spans="2:11">
       <c r="B62" s="4"/>
-      <c r="C62" s="11"/>
-      <c r="D62" s="11"/>
-      <c r="E62" s="11"/>
-      <c r="F62" s="11"/>
-      <c r="G62" s="11"/>
-      <c r="H62" s="11"/>
-      <c r="I62" s="11"/>
-      <c r="J62" s="11"/>
       <c r="K62" s="5"/>
     </row>
     <row r="63" spans="2:11">
       <c r="B63" s="4"/>
-      <c r="C63" s="11"/>
-      <c r="D63" s="11"/>
-      <c r="E63" s="11"/>
-      <c r="F63" s="11"/>
-      <c r="G63" s="11"/>
-      <c r="H63" s="11"/>
-      <c r="I63" s="11"/>
-      <c r="J63" s="11"/>
       <c r="K63" s="5"/>
     </row>
     <row r="64" spans="2:11">
       <c r="B64" s="4"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="11"/>
-      <c r="E64" s="11"/>
-      <c r="F64" s="11"/>
-      <c r="G64" s="11"/>
-      <c r="H64" s="11"/>
-      <c r="I64" s="11"/>
-      <c r="J64" s="11"/>
       <c r="K64" s="5"/>
     </row>
     <row r="65" spans="2:11">
       <c r="B65" s="4"/>
-      <c r="C65" s="11"/>
-      <c r="D65" s="11"/>
-      <c r="E65" s="11"/>
-      <c r="F65" s="11"/>
-      <c r="G65" s="11"/>
-      <c r="H65" s="11"/>
-      <c r="I65" s="11"/>
-      <c r="J65" s="11"/>
       <c r="K65" s="5"/>
     </row>
     <row r="66" spans="2:11">
       <c r="B66" s="4"/>
-      <c r="C66" s="11"/>
-      <c r="D66" s="11"/>
-      <c r="E66" s="11"/>
-      <c r="F66" s="11"/>
-      <c r="G66" s="11"/>
-      <c r="H66" s="11"/>
-      <c r="I66" s="11"/>
-      <c r="J66" s="11"/>
       <c r="K66" s="5"/>
     </row>
     <row r="67" spans="2:11">
       <c r="B67" s="4"/>
-      <c r="C67" s="11"/>
-      <c r="D67" s="11"/>
-      <c r="E67" s="11"/>
-      <c r="F67" s="11"/>
-      <c r="G67" s="11"/>
-      <c r="H67" s="11"/>
-      <c r="I67" s="11"/>
-      <c r="J67" s="11"/>
       <c r="K67" s="5"/>
     </row>
     <row r="68" spans="2:11">
       <c r="B68" s="4"/>
-      <c r="C68" s="11"/>
-      <c r="D68" s="11"/>
-      <c r="E68" s="11"/>
-      <c r="F68" s="11"/>
-      <c r="G68" s="11"/>
-      <c r="H68" s="11"/>
-      <c r="I68" s="11"/>
-      <c r="J68" s="11"/>
       <c r="K68" s="5"/>
     </row>
     <row r="69" spans="2:11">
       <c r="B69" s="4"/>
-      <c r="C69" s="11"/>
-      <c r="D69" s="11"/>
-      <c r="E69" s="11"/>
-      <c r="F69" s="11"/>
-      <c r="G69" s="11"/>
-      <c r="H69" s="11"/>
-      <c r="I69" s="11"/>
-      <c r="J69" s="11"/>
       <c r="K69" s="5"/>
     </row>
     <row r="70" spans="2:11">
@@ -2176,4 +2059,1945 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA31F806-B8EB-441F-B7AF-A95768670E04}">
+  <dimension ref="B3:S169"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="N63" sqref="N63"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetData>
+    <row r="3" spans="2:19">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="2:19">
+      <c r="B4" s="4"/>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="2:19">
+      <c r="B5" s="4"/>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="2:19">
+      <c r="B6" s="4"/>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="2:19">
+      <c r="B7" s="4"/>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="2:19">
+      <c r="B8" s="4"/>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="2:19">
+      <c r="B9" s="4"/>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="2:19">
+      <c r="B10" s="4"/>
+      <c r="E10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19">
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="9"/>
+    </row>
+    <row r="12" spans="2:19">
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+    </row>
+    <row r="13" spans="2:19">
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+    </row>
+    <row r="14" spans="2:19">
+      <c r="B14" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="3"/>
+    </row>
+    <row r="15" spans="2:19">
+      <c r="B15" s="15"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="5"/>
+    </row>
+    <row r="16" spans="2:19">
+      <c r="B16" s="15"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="5"/>
+    </row>
+    <row r="17" spans="2:19">
+      <c r="B17" s="15"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="5"/>
+    </row>
+    <row r="18" spans="2:19">
+      <c r="B18" s="15"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="5"/>
+    </row>
+    <row r="19" spans="2:19">
+      <c r="B19" s="15"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="5"/>
+    </row>
+    <row r="20" spans="2:19">
+      <c r="B20" s="15"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="11"/>
+      <c r="S20" s="5"/>
+    </row>
+    <row r="21" spans="2:19">
+      <c r="B21" s="15"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="5"/>
+    </row>
+    <row r="22" spans="2:19">
+      <c r="B22" s="15"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11"/>
+      <c r="S22" s="5"/>
+    </row>
+    <row r="23" spans="2:19">
+      <c r="B23" s="15"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="11"/>
+      <c r="S23" s="5"/>
+    </row>
+    <row r="24" spans="2:19">
+      <c r="B24" s="15"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="5"/>
+    </row>
+    <row r="25" spans="2:19">
+      <c r="B25" s="15"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="11"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="11"/>
+      <c r="S25" s="5"/>
+    </row>
+    <row r="26" spans="2:19">
+      <c r="B26" s="15"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="11"/>
+      <c r="R26" s="11"/>
+      <c r="S26" s="5"/>
+    </row>
+    <row r="27" spans="2:19">
+      <c r="B27" s="15"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="11"/>
+      <c r="R27" s="11"/>
+      <c r="S27" s="5"/>
+    </row>
+    <row r="28" spans="2:19">
+      <c r="B28" s="15"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="11"/>
+      <c r="S28" s="5"/>
+    </row>
+    <row r="29" spans="2:19">
+      <c r="B29" s="15"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="11"/>
+      <c r="P29" s="11"/>
+      <c r="Q29" s="11"/>
+      <c r="R29" s="11"/>
+      <c r="S29" s="5"/>
+    </row>
+    <row r="30" spans="2:19">
+      <c r="B30" s="15"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="11"/>
+      <c r="R30" s="11"/>
+      <c r="S30" s="5"/>
+    </row>
+    <row r="31" spans="2:19">
+      <c r="B31" s="15"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="11"/>
+      <c r="Q31" s="11"/>
+      <c r="R31" s="11"/>
+      <c r="S31" s="5"/>
+    </row>
+    <row r="32" spans="2:19">
+      <c r="B32" s="15"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="11"/>
+      <c r="P32" s="11"/>
+      <c r="Q32" s="11"/>
+      <c r="R32" s="11"/>
+      <c r="S32" s="5"/>
+    </row>
+    <row r="33" spans="2:19">
+      <c r="B33" s="15"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="11"/>
+      <c r="P33" s="11"/>
+      <c r="Q33" s="11"/>
+      <c r="R33" s="11"/>
+      <c r="S33" s="5"/>
+    </row>
+    <row r="34" spans="2:19">
+      <c r="B34" s="15"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="11"/>
+      <c r="O34" s="11"/>
+      <c r="P34" s="11"/>
+      <c r="Q34" s="11"/>
+      <c r="R34" s="11"/>
+      <c r="S34" s="5"/>
+    </row>
+    <row r="35" spans="2:19">
+      <c r="B35" s="15"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="11"/>
+      <c r="M35" s="11"/>
+      <c r="N35" s="11"/>
+      <c r="O35" s="11"/>
+      <c r="P35" s="11"/>
+      <c r="Q35" s="11"/>
+      <c r="R35" s="11"/>
+      <c r="S35" s="5"/>
+    </row>
+    <row r="36" spans="2:19">
+      <c r="B36" s="15"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11"/>
+      <c r="N36" s="11"/>
+      <c r="O36" s="11"/>
+      <c r="P36" s="11"/>
+      <c r="Q36" s="11"/>
+      <c r="R36" s="11"/>
+      <c r="S36" s="5"/>
+    </row>
+    <row r="37" spans="2:19">
+      <c r="B37" s="15"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="11"/>
+      <c r="M37" s="11"/>
+      <c r="N37" s="11"/>
+      <c r="O37" s="11"/>
+      <c r="P37" s="11"/>
+      <c r="Q37" s="11"/>
+      <c r="R37" s="11"/>
+      <c r="S37" s="5"/>
+    </row>
+    <row r="38" spans="2:19">
+      <c r="B38" s="15"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="11"/>
+      <c r="J38" s="11"/>
+      <c r="K38" s="11"/>
+      <c r="L38" s="11"/>
+      <c r="M38" s="11"/>
+      <c r="N38" s="11"/>
+      <c r="O38" s="11"/>
+      <c r="P38" s="11"/>
+      <c r="Q38" s="11"/>
+      <c r="R38" s="11"/>
+      <c r="S38" s="5"/>
+    </row>
+    <row r="39" spans="2:19">
+      <c r="B39" s="15"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="11"/>
+      <c r="L39" s="11"/>
+      <c r="M39" s="11"/>
+      <c r="N39" s="11"/>
+      <c r="O39" s="11"/>
+      <c r="P39" s="11"/>
+      <c r="Q39" s="11"/>
+      <c r="R39" s="11"/>
+      <c r="S39" s="5"/>
+    </row>
+    <row r="40" spans="2:19">
+      <c r="B40" s="15"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="11"/>
+      <c r="J40" s="11"/>
+      <c r="K40" s="11"/>
+      <c r="L40" s="11"/>
+      <c r="M40" s="11"/>
+      <c r="N40" s="11"/>
+      <c r="O40" s="11"/>
+      <c r="P40" s="11"/>
+      <c r="Q40" s="11"/>
+      <c r="R40" s="11"/>
+      <c r="S40" s="5"/>
+    </row>
+    <row r="41" spans="2:19">
+      <c r="B41" s="15"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="11"/>
+      <c r="K41" s="11"/>
+      <c r="L41" s="11"/>
+      <c r="M41" s="11"/>
+      <c r="N41" s="11"/>
+      <c r="O41" s="11"/>
+      <c r="P41" s="11"/>
+      <c r="Q41" s="11"/>
+      <c r="R41" s="11"/>
+      <c r="S41" s="5"/>
+    </row>
+    <row r="42" spans="2:19">
+      <c r="B42" s="15"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="11"/>
+      <c r="J42" s="11"/>
+      <c r="K42" s="11"/>
+      <c r="L42" s="11"/>
+      <c r="M42" s="11"/>
+      <c r="N42" s="11"/>
+      <c r="O42" s="11"/>
+      <c r="P42" s="11"/>
+      <c r="Q42" s="11"/>
+      <c r="R42" s="11"/>
+      <c r="S42" s="5"/>
+    </row>
+    <row r="43" spans="2:19">
+      <c r="B43" s="15"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="11"/>
+      <c r="J43" s="11"/>
+      <c r="K43" s="11"/>
+      <c r="L43" s="11"/>
+      <c r="M43" s="11"/>
+      <c r="N43" s="11"/>
+      <c r="O43" s="11"/>
+      <c r="P43" s="11"/>
+      <c r="Q43" s="11"/>
+      <c r="R43" s="11"/>
+      <c r="S43" s="5"/>
+    </row>
+    <row r="44" spans="2:19">
+      <c r="B44" s="16"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="8"/>
+      <c r="K44" s="8"/>
+      <c r="L44" s="8"/>
+      <c r="M44" s="8"/>
+      <c r="N44" s="8"/>
+      <c r="O44" s="8"/>
+      <c r="P44" s="8"/>
+      <c r="Q44" s="8"/>
+      <c r="R44" s="8"/>
+      <c r="S44" s="9"/>
+    </row>
+    <row r="45" spans="2:19">
+      <c r="B45" s="13"/>
+    </row>
+    <row r="46" spans="2:19">
+      <c r="B46" s="13"/>
+    </row>
+    <row r="47" spans="2:19">
+      <c r="B47" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="2:19">
+      <c r="B48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="3"/>
+    </row>
+    <row r="49" spans="2:13">
+      <c r="B49" s="4"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="11"/>
+      <c r="J49" s="11"/>
+      <c r="K49" s="5"/>
+    </row>
+    <row r="50" spans="2:13">
+      <c r="B50" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="11"/>
+      <c r="J50" s="11"/>
+      <c r="K50" s="5"/>
+    </row>
+    <row r="51" spans="2:13">
+      <c r="B51" s="4"/>
+      <c r="C51" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+      <c r="J51" s="11"/>
+      <c r="K51" s="5"/>
+    </row>
+    <row r="52" spans="2:13">
+      <c r="B52" s="4"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E52" s="12"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="11"/>
+      <c r="H52" s="11"/>
+      <c r="I52" s="11"/>
+      <c r="J52" s="11"/>
+      <c r="K52" s="5"/>
+    </row>
+    <row r="53" spans="2:13">
+      <c r="B53" s="4"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="12"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="11"/>
+      <c r="I53" s="11"/>
+      <c r="J53" s="11"/>
+      <c r="K53" s="5"/>
+    </row>
+    <row r="54" spans="2:13">
+      <c r="B54" s="4"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="11"/>
+      <c r="H54" s="11"/>
+      <c r="I54" s="11"/>
+      <c r="J54" s="11"/>
+      <c r="K54" s="5"/>
+    </row>
+    <row r="55" spans="2:13">
+      <c r="B55" s="4"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="11"/>
+      <c r="I55" s="11"/>
+      <c r="J55" s="11"/>
+      <c r="K55" s="5"/>
+    </row>
+    <row r="56" spans="2:13">
+      <c r="B56" s="4"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="11"/>
+      <c r="I56" s="11"/>
+      <c r="J56" s="11"/>
+      <c r="K56" s="5"/>
+    </row>
+    <row r="57" spans="2:13">
+      <c r="B57" s="4"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F57" s="12"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
+      <c r="I57" s="11"/>
+      <c r="J57" s="11"/>
+      <c r="K57" s="5"/>
+      <c r="L57" t="s">
+        <v>7</v>
+      </c>
+      <c r="M57" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="58" spans="2:13">
+      <c r="B58" s="4"/>
+      <c r="C58" s="11"/>
+      <c r="D58" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E58" s="12"/>
+      <c r="F58" s="12"/>
+      <c r="G58" s="11"/>
+      <c r="H58" s="11"/>
+      <c r="I58" s="11"/>
+      <c r="J58" s="11"/>
+      <c r="K58" s="5"/>
+    </row>
+    <row r="59" spans="2:13">
+      <c r="B59" s="4"/>
+      <c r="C59" s="11"/>
+      <c r="D59" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E59" s="12"/>
+      <c r="F59" s="12"/>
+      <c r="G59" s="11"/>
+      <c r="H59" s="11"/>
+      <c r="I59" s="11"/>
+      <c r="J59" s="11"/>
+      <c r="K59" s="5"/>
+    </row>
+    <row r="60" spans="2:13">
+      <c r="B60" s="4"/>
+      <c r="C60" s="11"/>
+      <c r="D60" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+      <c r="G60" s="11"/>
+      <c r="H60" s="11"/>
+      <c r="I60" s="11"/>
+      <c r="J60" s="11"/>
+      <c r="K60" s="5"/>
+    </row>
+    <row r="61" spans="2:13">
+      <c r="B61" s="4"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E61" s="12"/>
+      <c r="F61" s="12"/>
+      <c r="G61" s="11"/>
+      <c r="H61" s="11"/>
+      <c r="I61" s="11"/>
+      <c r="J61" s="11"/>
+      <c r="K61" s="5"/>
+    </row>
+    <row r="62" spans="2:13">
+      <c r="B62" s="4"/>
+      <c r="C62" s="11"/>
+      <c r="D62" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E62" s="12"/>
+      <c r="F62" s="12"/>
+      <c r="G62" s="11"/>
+      <c r="H62" s="11"/>
+      <c r="I62" s="11"/>
+      <c r="J62" s="11"/>
+      <c r="K62" s="5"/>
+    </row>
+    <row r="63" spans="2:13">
+      <c r="B63" s="4"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E63" s="12"/>
+      <c r="F63" s="12"/>
+      <c r="G63" s="11"/>
+      <c r="H63" s="11"/>
+      <c r="I63" s="11"/>
+      <c r="J63" s="11"/>
+      <c r="K63" s="5"/>
+    </row>
+    <row r="64" spans="2:13">
+      <c r="B64" s="4"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F64" s="12"/>
+      <c r="G64" s="11"/>
+      <c r="H64" s="11"/>
+      <c r="I64" s="11"/>
+      <c r="J64" s="11"/>
+      <c r="K64" s="5"/>
+    </row>
+    <row r="65" spans="2:11">
+      <c r="B65" s="4"/>
+      <c r="C65" s="11"/>
+      <c r="D65" s="12"/>
+      <c r="E65" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F65" s="12"/>
+      <c r="G65" s="11"/>
+      <c r="H65" s="11"/>
+      <c r="I65" s="11"/>
+      <c r="J65" s="11"/>
+      <c r="K65" s="5"/>
+    </row>
+    <row r="66" spans="2:11">
+      <c r="B66" s="4"/>
+      <c r="C66" s="11"/>
+      <c r="D66" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E66" s="12"/>
+      <c r="F66" s="12"/>
+      <c r="G66" s="11"/>
+      <c r="H66" s="11"/>
+      <c r="I66" s="11"/>
+      <c r="J66" s="11"/>
+      <c r="K66" s="5"/>
+    </row>
+    <row r="67" spans="2:11">
+      <c r="B67" s="4"/>
+      <c r="C67" s="11"/>
+      <c r="D67" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E67" s="12"/>
+      <c r="F67" s="12"/>
+      <c r="G67" s="11"/>
+      <c r="H67" s="11"/>
+      <c r="I67" s="11"/>
+      <c r="J67" s="11"/>
+      <c r="K67" s="5"/>
+    </row>
+    <row r="68" spans="2:11">
+      <c r="B68" s="4"/>
+      <c r="C68" s="11"/>
+      <c r="D68" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E68" s="12"/>
+      <c r="F68" s="12"/>
+      <c r="G68" s="11"/>
+      <c r="H68" s="11"/>
+      <c r="I68" s="11"/>
+      <c r="J68" s="11"/>
+      <c r="K68" s="5"/>
+    </row>
+    <row r="69" spans="2:11">
+      <c r="B69" s="4"/>
+      <c r="C69" s="11"/>
+      <c r="D69" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E69" s="12"/>
+      <c r="F69" s="12"/>
+      <c r="G69" s="11"/>
+      <c r="H69" s="11"/>
+      <c r="I69" s="11"/>
+      <c r="J69" s="11"/>
+      <c r="K69" s="5"/>
+    </row>
+    <row r="70" spans="2:11">
+      <c r="B70" s="4"/>
+      <c r="C70" s="11"/>
+      <c r="D70" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E70" s="12"/>
+      <c r="F70" s="12"/>
+      <c r="G70" s="11"/>
+      <c r="H70" s="11"/>
+      <c r="I70" s="11"/>
+      <c r="J70" s="11"/>
+      <c r="K70" s="5"/>
+    </row>
+    <row r="71" spans="2:11">
+      <c r="B71" s="4"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E71" s="12"/>
+      <c r="F71" s="12"/>
+      <c r="G71" s="11"/>
+      <c r="H71" s="11"/>
+      <c r="I71" s="11"/>
+      <c r="J71" s="11"/>
+      <c r="K71" s="5"/>
+    </row>
+    <row r="72" spans="2:11">
+      <c r="B72" s="4"/>
+      <c r="C72" s="11"/>
+      <c r="D72" s="12"/>
+      <c r="E72" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F72" s="12"/>
+      <c r="G72" s="11"/>
+      <c r="H72" s="11"/>
+      <c r="I72" s="11"/>
+      <c r="J72" s="11"/>
+      <c r="K72" s="5"/>
+    </row>
+    <row r="73" spans="2:11">
+      <c r="B73" s="4"/>
+      <c r="C73" s="11"/>
+      <c r="D73" s="12"/>
+      <c r="E73" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F73" s="12"/>
+      <c r="G73" s="11"/>
+      <c r="H73" s="11"/>
+      <c r="I73" s="11"/>
+      <c r="J73" s="11"/>
+      <c r="K73" s="5"/>
+    </row>
+    <row r="74" spans="2:11">
+      <c r="B74" s="4"/>
+      <c r="C74" s="11"/>
+      <c r="D74" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E74" s="12"/>
+      <c r="F74" s="12"/>
+      <c r="G74" s="11"/>
+      <c r="H74" s="11"/>
+      <c r="I74" s="11"/>
+      <c r="J74" s="11"/>
+      <c r="K74" s="5"/>
+    </row>
+    <row r="75" spans="2:11">
+      <c r="B75" s="4"/>
+      <c r="C75" s="11"/>
+      <c r="D75" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E75" s="12"/>
+      <c r="F75" s="12"/>
+      <c r="G75" s="11"/>
+      <c r="H75" s="11"/>
+      <c r="I75" s="11"/>
+      <c r="J75" s="11"/>
+      <c r="K75" s="5"/>
+    </row>
+    <row r="76" spans="2:11">
+      <c r="B76" s="4"/>
+      <c r="C76" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D76" s="11"/>
+      <c r="E76" s="11"/>
+      <c r="F76" s="11"/>
+      <c r="G76" s="11"/>
+      <c r="H76" s="11"/>
+      <c r="I76" s="11"/>
+      <c r="J76" s="11"/>
+      <c r="K76" s="5"/>
+    </row>
+    <row r="77" spans="2:11">
+      <c r="B77" s="4"/>
+      <c r="C77" s="11"/>
+      <c r="D77" s="11"/>
+      <c r="E77" s="11"/>
+      <c r="F77" s="11"/>
+      <c r="G77" s="11"/>
+      <c r="H77" s="11"/>
+      <c r="I77" s="11"/>
+      <c r="J77" s="11"/>
+      <c r="K77" s="5"/>
+    </row>
+    <row r="78" spans="2:11">
+      <c r="B78" s="4"/>
+      <c r="C78" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D78" s="11"/>
+      <c r="E78" s="11"/>
+      <c r="F78" s="11"/>
+      <c r="G78" s="11"/>
+      <c r="H78" s="11"/>
+      <c r="I78" s="11"/>
+      <c r="J78" s="11"/>
+      <c r="K78" s="5"/>
+    </row>
+    <row r="79" spans="2:11">
+      <c r="B79" s="4"/>
+      <c r="C79" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D79" s="11"/>
+      <c r="E79" s="11"/>
+      <c r="F79" s="11"/>
+      <c r="G79" s="11"/>
+      <c r="H79" s="11"/>
+      <c r="I79" s="11"/>
+      <c r="J79" s="11"/>
+      <c r="K79" s="5"/>
+    </row>
+    <row r="80" spans="2:11">
+      <c r="B80" s="4"/>
+      <c r="C80" s="11"/>
+      <c r="D80" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E80" s="11"/>
+      <c r="F80" s="11"/>
+      <c r="G80" s="11"/>
+      <c r="H80" s="11"/>
+      <c r="I80" s="11"/>
+      <c r="J80" s="11"/>
+      <c r="K80" s="5"/>
+    </row>
+    <row r="81" spans="2:11">
+      <c r="B81" s="4"/>
+      <c r="C81" s="11"/>
+      <c r="D81" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E81" s="11"/>
+      <c r="F81" s="11"/>
+      <c r="G81" s="11"/>
+      <c r="H81" s="11"/>
+      <c r="I81" s="11"/>
+      <c r="J81" s="11"/>
+      <c r="K81" s="5"/>
+    </row>
+    <row r="82" spans="2:11">
+      <c r="B82" s="4"/>
+      <c r="C82" s="11"/>
+      <c r="D82" s="11"/>
+      <c r="E82" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F82" s="11"/>
+      <c r="G82" s="11"/>
+      <c r="H82" s="11"/>
+      <c r="I82" s="11"/>
+      <c r="J82" s="11"/>
+      <c r="K82" s="5"/>
+    </row>
+    <row r="83" spans="2:11">
+      <c r="B83" s="4"/>
+      <c r="C83" s="11"/>
+      <c r="D83" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E83" s="11"/>
+      <c r="F83" s="11"/>
+      <c r="G83" s="11"/>
+      <c r="H83" s="11"/>
+      <c r="I83" s="11"/>
+      <c r="J83" s="11"/>
+      <c r="K83" s="5"/>
+    </row>
+    <row r="84" spans="2:11">
+      <c r="B84" s="4"/>
+      <c r="C84" s="11"/>
+      <c r="D84" s="11"/>
+      <c r="E84" s="11"/>
+      <c r="F84" s="11"/>
+      <c r="G84" s="11"/>
+      <c r="H84" s="11"/>
+      <c r="I84" s="11"/>
+      <c r="J84" s="11"/>
+      <c r="K84" s="5"/>
+    </row>
+    <row r="85" spans="2:11">
+      <c r="B85" s="4"/>
+      <c r="C85" s="11"/>
+      <c r="D85" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E85" s="11"/>
+      <c r="F85" s="11"/>
+      <c r="G85" s="11"/>
+      <c r="H85" s="11"/>
+      <c r="I85" s="11"/>
+      <c r="J85" s="11"/>
+      <c r="K85" s="5"/>
+    </row>
+    <row r="86" spans="2:11">
+      <c r="B86" s="4"/>
+      <c r="C86" s="11"/>
+      <c r="D86" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E86" s="11"/>
+      <c r="F86" s="11"/>
+      <c r="G86" s="11"/>
+      <c r="H86" s="11"/>
+      <c r="I86" s="11"/>
+      <c r="J86" s="11"/>
+      <c r="K86" s="5"/>
+    </row>
+    <row r="87" spans="2:11">
+      <c r="B87" s="4"/>
+      <c r="C87" s="11"/>
+      <c r="D87" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E87" s="11"/>
+      <c r="F87" s="11"/>
+      <c r="G87" s="11"/>
+      <c r="H87" s="11"/>
+      <c r="I87" s="11"/>
+      <c r="J87" s="11"/>
+      <c r="K87" s="5"/>
+    </row>
+    <row r="88" spans="2:11">
+      <c r="B88" s="4"/>
+      <c r="C88" s="11"/>
+      <c r="D88" s="11"/>
+      <c r="E88" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F88" s="11"/>
+      <c r="G88" s="11"/>
+      <c r="H88" s="11"/>
+      <c r="I88" s="11"/>
+      <c r="J88" s="11"/>
+      <c r="K88" s="5"/>
+    </row>
+    <row r="89" spans="2:11">
+      <c r="B89" s="4"/>
+      <c r="C89" s="11"/>
+      <c r="D89" s="11"/>
+      <c r="E89" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F89" s="11"/>
+      <c r="G89" s="11"/>
+      <c r="H89" s="11"/>
+      <c r="I89" s="11"/>
+      <c r="J89" s="11"/>
+      <c r="K89" s="5"/>
+    </row>
+    <row r="90" spans="2:11">
+      <c r="B90" s="4"/>
+      <c r="C90" s="11"/>
+      <c r="D90" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E90" s="11"/>
+      <c r="F90" s="11"/>
+      <c r="G90" s="11"/>
+      <c r="H90" s="11"/>
+      <c r="I90" s="11"/>
+      <c r="J90" s="11"/>
+      <c r="K90" s="5"/>
+    </row>
+    <row r="91" spans="2:11">
+      <c r="B91" s="4"/>
+      <c r="C91" s="11"/>
+      <c r="D91" s="11"/>
+      <c r="E91" s="11"/>
+      <c r="F91" s="11"/>
+      <c r="G91" s="11"/>
+      <c r="H91" s="11"/>
+      <c r="I91" s="11"/>
+      <c r="J91" s="11"/>
+      <c r="K91" s="5"/>
+    </row>
+    <row r="92" spans="2:11">
+      <c r="B92" s="4"/>
+      <c r="C92" s="11"/>
+      <c r="D92" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E92" s="11"/>
+      <c r="F92" s="11"/>
+      <c r="G92" s="11"/>
+      <c r="H92" s="11"/>
+      <c r="I92" s="11"/>
+      <c r="J92" s="11"/>
+      <c r="K92" s="5"/>
+    </row>
+    <row r="93" spans="2:11">
+      <c r="B93" s="4"/>
+      <c r="C93" s="11"/>
+      <c r="D93" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E93" s="11"/>
+      <c r="F93" s="11"/>
+      <c r="G93" s="11"/>
+      <c r="H93" s="11"/>
+      <c r="I93" s="11"/>
+      <c r="J93" s="11"/>
+      <c r="K93" s="5"/>
+    </row>
+    <row r="94" spans="2:11">
+      <c r="B94" s="4"/>
+      <c r="C94" s="11"/>
+      <c r="D94" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E94" s="11"/>
+      <c r="F94" s="11"/>
+      <c r="G94" s="11"/>
+      <c r="H94" s="11"/>
+      <c r="I94" s="11"/>
+      <c r="J94" s="11"/>
+      <c r="K94" s="5"/>
+    </row>
+    <row r="95" spans="2:11">
+      <c r="B95" s="4"/>
+      <c r="C95" s="11"/>
+      <c r="D95" s="11"/>
+      <c r="E95" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F95" s="11"/>
+      <c r="G95" s="11"/>
+      <c r="H95" s="11"/>
+      <c r="I95" s="11"/>
+      <c r="J95" s="11"/>
+      <c r="K95" s="5"/>
+    </row>
+    <row r="96" spans="2:11">
+      <c r="B96" s="4"/>
+      <c r="C96" s="11"/>
+      <c r="D96" s="11"/>
+      <c r="E96" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F96" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G96" s="11"/>
+      <c r="H96" s="11"/>
+      <c r="I96" s="11"/>
+      <c r="J96" s="11"/>
+      <c r="K96" s="5"/>
+    </row>
+    <row r="97" spans="2:11">
+      <c r="B97" s="4"/>
+      <c r="C97" s="11"/>
+      <c r="D97" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E97" s="11"/>
+      <c r="F97" s="11"/>
+      <c r="G97" s="11"/>
+      <c r="H97" s="11"/>
+      <c r="I97" s="11"/>
+      <c r="J97" s="11"/>
+      <c r="K97" s="5"/>
+    </row>
+    <row r="98" spans="2:11">
+      <c r="B98" s="4"/>
+      <c r="C98" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D98" s="11"/>
+      <c r="E98" s="11"/>
+      <c r="F98" s="11"/>
+      <c r="G98" s="11"/>
+      <c r="H98" s="11"/>
+      <c r="I98" s="11"/>
+      <c r="J98" s="11"/>
+      <c r="K98" s="5"/>
+    </row>
+    <row r="99" spans="2:11">
+      <c r="B99" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C99" s="11"/>
+      <c r="D99" s="11"/>
+      <c r="E99" s="11"/>
+      <c r="F99" s="11"/>
+      <c r="G99" s="11"/>
+      <c r="H99" s="11"/>
+      <c r="I99" s="11"/>
+      <c r="J99" s="11"/>
+      <c r="K99" s="5"/>
+    </row>
+    <row r="100" spans="2:11">
+      <c r="B100" s="7"/>
+      <c r="C100" s="8"/>
+      <c r="D100" s="8"/>
+      <c r="E100" s="8"/>
+      <c r="F100" s="8"/>
+      <c r="G100" s="8"/>
+      <c r="H100" s="8"/>
+      <c r="I100" s="8"/>
+      <c r="J100" s="8"/>
+      <c r="K100" s="9"/>
+    </row>
+    <row r="137" spans="2:13">
+      <c r="B137" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C137" s="2"/>
+      <c r="D137" s="2"/>
+      <c r="E137" s="2"/>
+      <c r="F137" s="2"/>
+      <c r="G137" s="2"/>
+      <c r="H137" s="2"/>
+      <c r="I137" s="2"/>
+      <c r="J137" s="2"/>
+      <c r="K137" s="2"/>
+      <c r="L137" s="2"/>
+      <c r="M137" s="3"/>
+    </row>
+    <row r="138" spans="2:13">
+      <c r="B138" s="4"/>
+      <c r="C138" s="11"/>
+      <c r="D138" s="11"/>
+      <c r="E138" s="11"/>
+      <c r="F138" s="11"/>
+      <c r="G138" s="11"/>
+      <c r="H138" s="11"/>
+      <c r="I138" s="11"/>
+      <c r="J138" s="11"/>
+      <c r="K138" s="11"/>
+      <c r="L138" s="11"/>
+      <c r="M138" s="5"/>
+    </row>
+    <row r="139" spans="2:13">
+      <c r="B139" s="4"/>
+      <c r="C139" s="11"/>
+      <c r="D139" s="11"/>
+      <c r="E139" s="11"/>
+      <c r="F139" s="11"/>
+      <c r="G139" s="11"/>
+      <c r="H139" s="11"/>
+      <c r="I139" s="11"/>
+      <c r="J139" s="11"/>
+      <c r="K139" s="11"/>
+      <c r="L139" s="11"/>
+      <c r="M139" s="5"/>
+    </row>
+    <row r="140" spans="2:13">
+      <c r="B140" s="4"/>
+      <c r="C140" s="11"/>
+      <c r="D140" s="11"/>
+      <c r="E140" s="11"/>
+      <c r="F140" s="11"/>
+      <c r="G140" s="11"/>
+      <c r="H140" s="11"/>
+      <c r="I140" s="11"/>
+      <c r="J140" s="11"/>
+      <c r="K140" s="11"/>
+      <c r="L140" s="11"/>
+      <c r="M140" s="5"/>
+    </row>
+    <row r="141" spans="2:13">
+      <c r="B141" s="4"/>
+      <c r="C141" s="11"/>
+      <c r="D141" s="11"/>
+      <c r="E141" s="11"/>
+      <c r="F141" s="11"/>
+      <c r="G141" s="11"/>
+      <c r="H141" s="11"/>
+      <c r="I141" s="11"/>
+      <c r="J141" s="11"/>
+      <c r="K141" s="11"/>
+      <c r="L141" s="11"/>
+      <c r="M141" s="5"/>
+    </row>
+    <row r="142" spans="2:13">
+      <c r="B142" s="4"/>
+      <c r="C142" s="11"/>
+      <c r="D142" s="11"/>
+      <c r="E142" s="11"/>
+      <c r="F142" s="11"/>
+      <c r="G142" s="11"/>
+      <c r="H142" s="11"/>
+      <c r="I142" s="11"/>
+      <c r="J142" s="11"/>
+      <c r="K142" s="11"/>
+      <c r="L142" s="11"/>
+      <c r="M142" s="5"/>
+    </row>
+    <row r="143" spans="2:13">
+      <c r="B143" s="4"/>
+      <c r="C143" s="11"/>
+      <c r="D143" s="11"/>
+      <c r="E143" s="11"/>
+      <c r="F143" s="11"/>
+      <c r="G143" s="11"/>
+      <c r="H143" s="11"/>
+      <c r="I143" s="11"/>
+      <c r="J143" s="11"/>
+      <c r="K143" s="11"/>
+      <c r="L143" s="11"/>
+      <c r="M143" s="5"/>
+    </row>
+    <row r="144" spans="2:13">
+      <c r="B144" s="4"/>
+      <c r="C144" s="11"/>
+      <c r="D144" s="11"/>
+      <c r="E144" s="11"/>
+      <c r="F144" s="11"/>
+      <c r="G144" s="11"/>
+      <c r="H144" s="11"/>
+      <c r="I144" s="11"/>
+      <c r="J144" s="11"/>
+      <c r="K144" s="11"/>
+      <c r="L144" s="11"/>
+      <c r="M144" s="5"/>
+    </row>
+    <row r="145" spans="2:13">
+      <c r="B145" s="4"/>
+      <c r="C145" s="11"/>
+      <c r="D145" s="11"/>
+      <c r="E145" s="11"/>
+      <c r="F145" s="11"/>
+      <c r="G145" s="11"/>
+      <c r="H145" s="11"/>
+      <c r="I145" s="11"/>
+      <c r="J145" s="11"/>
+      <c r="K145" s="11"/>
+      <c r="L145" s="11"/>
+      <c r="M145" s="5"/>
+    </row>
+    <row r="146" spans="2:13">
+      <c r="B146" s="4"/>
+      <c r="C146" s="11"/>
+      <c r="D146" s="11"/>
+      <c r="E146" s="11"/>
+      <c r="F146" s="11"/>
+      <c r="G146" s="11"/>
+      <c r="H146" s="11"/>
+      <c r="I146" s="11"/>
+      <c r="J146" s="11"/>
+      <c r="K146" s="11"/>
+      <c r="L146" s="11"/>
+      <c r="M146" s="5"/>
+    </row>
+    <row r="147" spans="2:13">
+      <c r="B147" s="4"/>
+      <c r="C147" s="11"/>
+      <c r="D147" s="11"/>
+      <c r="E147" s="11"/>
+      <c r="F147" s="11"/>
+      <c r="G147" s="11"/>
+      <c r="H147" s="11"/>
+      <c r="I147" s="11"/>
+      <c r="J147" s="11"/>
+      <c r="K147" s="11"/>
+      <c r="L147" s="11"/>
+      <c r="M147" s="5"/>
+    </row>
+    <row r="148" spans="2:13">
+      <c r="B148" s="4"/>
+      <c r="C148" s="11"/>
+      <c r="D148" s="11"/>
+      <c r="E148" s="11"/>
+      <c r="F148" s="11"/>
+      <c r="G148" s="11"/>
+      <c r="H148" s="11"/>
+      <c r="I148" s="11"/>
+      <c r="J148" s="11"/>
+      <c r="K148" s="11"/>
+      <c r="L148" s="11"/>
+      <c r="M148" s="5"/>
+    </row>
+    <row r="149" spans="2:13">
+      <c r="B149" s="4"/>
+      <c r="C149" s="11"/>
+      <c r="D149" s="11"/>
+      <c r="E149" s="11"/>
+      <c r="F149" s="11"/>
+      <c r="G149" s="11"/>
+      <c r="H149" s="11"/>
+      <c r="I149" s="11"/>
+      <c r="J149" s="11"/>
+      <c r="K149" s="11"/>
+      <c r="L149" s="11"/>
+      <c r="M149" s="5"/>
+    </row>
+    <row r="150" spans="2:13">
+      <c r="B150" s="4"/>
+      <c r="C150" s="11"/>
+      <c r="D150" s="11"/>
+      <c r="E150" s="11"/>
+      <c r="F150" s="11"/>
+      <c r="G150" s="11"/>
+      <c r="H150" s="11"/>
+      <c r="I150" s="11"/>
+      <c r="J150" s="11"/>
+      <c r="K150" s="11"/>
+      <c r="L150" s="11"/>
+      <c r="M150" s="5"/>
+    </row>
+    <row r="151" spans="2:13">
+      <c r="B151" s="4"/>
+      <c r="C151" s="11"/>
+      <c r="D151" s="11"/>
+      <c r="E151" s="11"/>
+      <c r="F151" s="11"/>
+      <c r="G151" s="11"/>
+      <c r="H151" s="11"/>
+      <c r="I151" s="11"/>
+      <c r="J151" s="11"/>
+      <c r="K151" s="11"/>
+      <c r="L151" s="11"/>
+      <c r="M151" s="5"/>
+    </row>
+    <row r="152" spans="2:13">
+      <c r="B152" s="4"/>
+      <c r="C152" s="11"/>
+      <c r="D152" s="11"/>
+      <c r="E152" s="11"/>
+      <c r="F152" s="11"/>
+      <c r="G152" s="11"/>
+      <c r="H152" s="11"/>
+      <c r="I152" s="11"/>
+      <c r="J152" s="11"/>
+      <c r="K152" s="11"/>
+      <c r="L152" s="11"/>
+      <c r="M152" s="5"/>
+    </row>
+    <row r="153" spans="2:13">
+      <c r="B153" s="4"/>
+      <c r="C153" s="11"/>
+      <c r="D153" s="11"/>
+      <c r="E153" s="11"/>
+      <c r="F153" s="11"/>
+      <c r="G153" s="11"/>
+      <c r="H153" s="11"/>
+      <c r="I153" s="11"/>
+      <c r="J153" s="11"/>
+      <c r="K153" s="11"/>
+      <c r="L153" s="11"/>
+      <c r="M153" s="5"/>
+    </row>
+    <row r="154" spans="2:13">
+      <c r="B154" s="4"/>
+      <c r="C154" s="11"/>
+      <c r="D154" s="11"/>
+      <c r="E154" s="11"/>
+      <c r="F154" s="11"/>
+      <c r="G154" s="11"/>
+      <c r="H154" s="11"/>
+      <c r="I154" s="11"/>
+      <c r="J154" s="11"/>
+      <c r="K154" s="11"/>
+      <c r="L154" s="11"/>
+      <c r="M154" s="5"/>
+    </row>
+    <row r="155" spans="2:13">
+      <c r="B155" s="4"/>
+      <c r="C155" s="11"/>
+      <c r="D155" s="11"/>
+      <c r="E155" s="11"/>
+      <c r="F155" s="11"/>
+      <c r="G155" s="11"/>
+      <c r="H155" s="11"/>
+      <c r="I155" s="11"/>
+      <c r="J155" s="11"/>
+      <c r="K155" s="11"/>
+      <c r="L155" s="11"/>
+      <c r="M155" s="5"/>
+    </row>
+    <row r="156" spans="2:13">
+      <c r="B156" s="4"/>
+      <c r="C156" s="11"/>
+      <c r="D156" s="11"/>
+      <c r="E156" s="11"/>
+      <c r="F156" s="11"/>
+      <c r="G156" s="11"/>
+      <c r="H156" s="11"/>
+      <c r="I156" s="11"/>
+      <c r="J156" s="11"/>
+      <c r="K156" s="11"/>
+      <c r="L156" s="11"/>
+      <c r="M156" s="5"/>
+    </row>
+    <row r="157" spans="2:13">
+      <c r="B157" s="4"/>
+      <c r="C157" s="11"/>
+      <c r="D157" s="11"/>
+      <c r="E157" s="11"/>
+      <c r="F157" s="11"/>
+      <c r="G157" s="11"/>
+      <c r="H157" s="11"/>
+      <c r="I157" s="11"/>
+      <c r="J157" s="11"/>
+      <c r="K157" s="11"/>
+      <c r="L157" s="11"/>
+      <c r="M157" s="5"/>
+    </row>
+    <row r="158" spans="2:13">
+      <c r="B158" s="4"/>
+      <c r="C158" s="11"/>
+      <c r="D158" s="11"/>
+      <c r="E158" s="11"/>
+      <c r="F158" s="11"/>
+      <c r="G158" s="11"/>
+      <c r="H158" s="11"/>
+      <c r="I158" s="11"/>
+      <c r="J158" s="11"/>
+      <c r="K158" s="11"/>
+      <c r="L158" s="11"/>
+      <c r="M158" s="5"/>
+    </row>
+    <row r="159" spans="2:13">
+      <c r="B159" s="4"/>
+      <c r="C159" s="11"/>
+      <c r="D159" s="11"/>
+      <c r="E159" s="11"/>
+      <c r="F159" s="11"/>
+      <c r="G159" s="11"/>
+      <c r="H159" s="11"/>
+      <c r="I159" s="11"/>
+      <c r="J159" s="11"/>
+      <c r="K159" s="11"/>
+      <c r="L159" s="11"/>
+      <c r="M159" s="5"/>
+    </row>
+    <row r="160" spans="2:13">
+      <c r="B160" s="4"/>
+      <c r="C160" s="11"/>
+      <c r="D160" s="11"/>
+      <c r="E160" s="11"/>
+      <c r="F160" s="11"/>
+      <c r="G160" s="11"/>
+      <c r="H160" s="11"/>
+      <c r="I160" s="11"/>
+      <c r="J160" s="11"/>
+      <c r="K160" s="11"/>
+      <c r="L160" s="11"/>
+      <c r="M160" s="5"/>
+    </row>
+    <row r="161" spans="2:13">
+      <c r="B161" s="4"/>
+      <c r="C161" s="11"/>
+      <c r="D161" s="11"/>
+      <c r="E161" s="11"/>
+      <c r="F161" s="11"/>
+      <c r="G161" s="11"/>
+      <c r="H161" s="11"/>
+      <c r="I161" s="11"/>
+      <c r="J161" s="11"/>
+      <c r="K161" s="11"/>
+      <c r="L161" s="11"/>
+      <c r="M161" s="5"/>
+    </row>
+    <row r="162" spans="2:13">
+      <c r="B162" s="4"/>
+      <c r="C162" s="11"/>
+      <c r="D162" s="11"/>
+      <c r="E162" s="11"/>
+      <c r="F162" s="11"/>
+      <c r="G162" s="11"/>
+      <c r="H162" s="11"/>
+      <c r="I162" s="11"/>
+      <c r="J162" s="11"/>
+      <c r="K162" s="11"/>
+      <c r="L162" s="11"/>
+      <c r="M162" s="5"/>
+    </row>
+    <row r="163" spans="2:13">
+      <c r="B163" s="4"/>
+      <c r="C163" s="11"/>
+      <c r="D163" s="11"/>
+      <c r="E163" s="11"/>
+      <c r="F163" s="11"/>
+      <c r="G163" s="11"/>
+      <c r="H163" s="11"/>
+      <c r="I163" s="11"/>
+      <c r="J163" s="11"/>
+      <c r="K163" s="11"/>
+      <c r="L163" s="11"/>
+      <c r="M163" s="5"/>
+    </row>
+    <row r="164" spans="2:13">
+      <c r="B164" s="4"/>
+      <c r="C164" s="11"/>
+      <c r="D164" s="11"/>
+      <c r="E164" s="11"/>
+      <c r="F164" s="11"/>
+      <c r="G164" s="11"/>
+      <c r="H164" s="11"/>
+      <c r="I164" s="11"/>
+      <c r="J164" s="11"/>
+      <c r="K164" s="11"/>
+      <c r="L164" s="11"/>
+      <c r="M164" s="5"/>
+    </row>
+    <row r="165" spans="2:13">
+      <c r="B165" s="4"/>
+      <c r="C165" s="11"/>
+      <c r="D165" s="11"/>
+      <c r="E165" s="11"/>
+      <c r="F165" s="11"/>
+      <c r="G165" s="11"/>
+      <c r="H165" s="11"/>
+      <c r="I165" s="11"/>
+      <c r="J165" s="11"/>
+      <c r="K165" s="11"/>
+      <c r="L165" s="11"/>
+      <c r="M165" s="5"/>
+    </row>
+    <row r="166" spans="2:13">
+      <c r="B166" s="4"/>
+      <c r="C166" s="11"/>
+      <c r="D166" s="11"/>
+      <c r="E166" s="11"/>
+      <c r="F166" s="11"/>
+      <c r="G166" s="11"/>
+      <c r="H166" s="11"/>
+      <c r="I166" s="11"/>
+      <c r="J166" s="11"/>
+      <c r="K166" s="11"/>
+      <c r="L166" s="11"/>
+      <c r="M166" s="5"/>
+    </row>
+    <row r="167" spans="2:13">
+      <c r="B167" s="4"/>
+      <c r="C167" s="11"/>
+      <c r="D167" s="11"/>
+      <c r="E167" s="11"/>
+      <c r="F167" s="11"/>
+      <c r="G167" s="11"/>
+      <c r="H167" s="11"/>
+      <c r="I167" s="11"/>
+      <c r="J167" s="11"/>
+      <c r="K167" s="11"/>
+      <c r="L167" s="11"/>
+      <c r="M167" s="5"/>
+    </row>
+    <row r="168" spans="2:13">
+      <c r="B168" s="4"/>
+      <c r="C168" s="11"/>
+      <c r="D168" s="11"/>
+      <c r="E168" s="11"/>
+      <c r="F168" s="11"/>
+      <c r="G168" s="11"/>
+      <c r="H168" s="11"/>
+      <c r="I168" s="11"/>
+      <c r="J168" s="11"/>
+      <c r="K168" s="11"/>
+      <c r="L168" s="11"/>
+      <c r="M168" s="5"/>
+    </row>
+    <row r="169" spans="2:13">
+      <c r="B169" s="7"/>
+      <c r="C169" s="8"/>
+      <c r="D169" s="8"/>
+      <c r="E169" s="8"/>
+      <c r="F169" s="8"/>
+      <c r="G169" s="8"/>
+      <c r="H169" s="8"/>
+      <c r="I169" s="8"/>
+      <c r="J169" s="8"/>
+      <c r="K169" s="8"/>
+      <c r="L169" s="8"/>
+      <c r="M169" s="9"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Ex Bảng cửu chương _ Full
</commit_message>
<xml_diff>
--- a/1.nen-tang-lap-trinh-java/5.vong-lap.xlsx
+++ b/1.nen-tang-lap-trinh-java/5.vong-lap.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\java\1.nen-tang-lap-trinh-java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A77765C4-8ECA-46C3-928E-0287E1CF528A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905C1D2D-6E3C-40DA-B4AF-72F21F78082D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30225" yWindow="1050" windowWidth="26070" windowHeight="13830" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30225" yWindow="1050" windowWidth="26070" windowHeight="13830" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vòng lặp" sheetId="1" r:id="rId1"/>
     <sheet name="Ex Bảng cửu chương _ Basic" sheetId="2" r:id="rId2"/>
+    <sheet name="Ex Bảng cửu chương _ Full" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="60">
   <si>
     <t>java_training</t>
     <phoneticPr fontId="1"/>
@@ -775,6 +776,108 @@
   </si>
   <si>
     <t>https://docs.oracle.com/javase/tutorial/java/data/numberformat.html</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>int i = 2;</t>
+  </si>
+  <si>
+    <t>while(i &lt;= 9){</t>
+  </si>
+  <si>
+    <t>for(int j = 1; j &lt;= 10; j++){</t>
+  </si>
+  <si>
+    <t>System.out.printf("%d x %d = %d%n", i, j, i*j);</t>
+  </si>
+  <si>
+    <t>i++;</t>
+  </si>
+  <si>
+    <r>
+      <t>// 002 BẢNG CỬU CH</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ƯƠ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NG - BASIC</t>
+    </r>
+  </si>
+  <si>
+    <t>public static void main002(String[] args) {</t>
+  </si>
+  <si>
+    <t>System.out.printf("%d x %d = %d%n", number, i, number*i);</t>
+  </si>
+  <si>
+    <r>
+      <t>System.out.println("Bảng cửu ch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ươ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ng " + i);</t>
+    </r>
+  </si>
+  <si>
+    <t>System.out.println();</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>1 dòng tr</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>ắ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ng</t>
+    </r>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -782,7 +885,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -824,6 +927,21 @@
       <name val="Segoe UI"/>
       <family val="2"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Yu Gothic"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Yu Gothic"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -932,7 +1050,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -944,12 +1062,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1365,6 +1484,99 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>143863</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="図 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76D92408-49F8-5706-6FB6-751418858E85}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="809625" y="18630900"/>
+          <a:ext cx="13877925" cy="6433538"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>494438</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>113295</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="図 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48275B29-AC5A-D8B6-723E-A0ABF0D099D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="828675" y="25679400"/>
+          <a:ext cx="6895238" cy="8038095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2065,8 +2277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA31F806-B8EB-441F-B7AF-A95768670E04}">
   <dimension ref="B3:S169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="N63" sqref="N63"/>
+    <sheetView topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="Q148" sqref="Q148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -2144,24 +2356,8 @@
       <c r="F11" s="8"/>
       <c r="G11" s="9"/>
     </row>
-    <row r="12" spans="2:19">
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-    </row>
-    <row r="13" spans="2:19">
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-    </row>
     <row r="14" spans="2:19">
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="12" t="s">
         <v>48</v>
       </c>
       <c r="C14" s="2"/>
@@ -2183,587 +2379,123 @@
       <c r="S14" s="3"/>
     </row>
     <row r="15" spans="2:19">
-      <c r="B15" s="15"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="11"/>
-      <c r="R15" s="11"/>
+      <c r="B15" s="13"/>
       <c r="S15" s="5"/>
     </row>
     <row r="16" spans="2:19">
-      <c r="B16" s="15"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="11"/>
-      <c r="O16" s="11"/>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="11"/>
-      <c r="R16" s="11"/>
+      <c r="B16" s="13"/>
       <c r="S16" s="5"/>
     </row>
     <row r="17" spans="2:19">
-      <c r="B17" s="15"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="11"/>
-      <c r="O17" s="11"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="11"/>
-      <c r="R17" s="11"/>
+      <c r="B17" s="13"/>
       <c r="S17" s="5"/>
     </row>
     <row r="18" spans="2:19">
-      <c r="B18" s="15"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="11"/>
-      <c r="N18" s="11"/>
-      <c r="O18" s="11"/>
-      <c r="P18" s="11"/>
-      <c r="Q18" s="11"/>
-      <c r="R18" s="11"/>
+      <c r="B18" s="13"/>
       <c r="S18" s="5"/>
     </row>
     <row r="19" spans="2:19">
-      <c r="B19" s="15"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
-      <c r="N19" s="11"/>
-      <c r="O19" s="11"/>
-      <c r="P19" s="11"/>
-      <c r="Q19" s="11"/>
-      <c r="R19" s="11"/>
+      <c r="B19" s="13"/>
       <c r="S19" s="5"/>
     </row>
     <row r="20" spans="2:19">
-      <c r="B20" s="15"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="11"/>
-      <c r="N20" s="11"/>
-      <c r="O20" s="11"/>
-      <c r="P20" s="11"/>
-      <c r="Q20" s="11"/>
-      <c r="R20" s="11"/>
+      <c r="B20" s="13"/>
       <c r="S20" s="5"/>
     </row>
     <row r="21" spans="2:19">
-      <c r="B21" s="15"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
-      <c r="N21" s="11"/>
-      <c r="O21" s="11"/>
-      <c r="P21" s="11"/>
-      <c r="Q21" s="11"/>
-      <c r="R21" s="11"/>
+      <c r="B21" s="13"/>
       <c r="S21" s="5"/>
     </row>
     <row r="22" spans="2:19">
-      <c r="B22" s="15"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
-      <c r="N22" s="11"/>
-      <c r="O22" s="11"/>
-      <c r="P22" s="11"/>
-      <c r="Q22" s="11"/>
-      <c r="R22" s="11"/>
+      <c r="B22" s="13"/>
       <c r="S22" s="5"/>
     </row>
     <row r="23" spans="2:19">
-      <c r="B23" s="15"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
-      <c r="L23" s="11"/>
-      <c r="M23" s="11"/>
-      <c r="N23" s="11"/>
-      <c r="O23" s="11"/>
-      <c r="P23" s="11"/>
-      <c r="Q23" s="11"/>
-      <c r="R23" s="11"/>
+      <c r="B23" s="13"/>
       <c r="S23" s="5"/>
     </row>
     <row r="24" spans="2:19">
-      <c r="B24" s="15"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="11"/>
-      <c r="N24" s="11"/>
-      <c r="O24" s="11"/>
-      <c r="P24" s="11"/>
-      <c r="Q24" s="11"/>
-      <c r="R24" s="11"/>
+      <c r="B24" s="13"/>
       <c r="S24" s="5"/>
     </row>
     <row r="25" spans="2:19">
-      <c r="B25" s="15"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
-      <c r="M25" s="11"/>
-      <c r="N25" s="11"/>
-      <c r="O25" s="11"/>
-      <c r="P25" s="11"/>
-      <c r="Q25" s="11"/>
-      <c r="R25" s="11"/>
+      <c r="B25" s="13"/>
       <c r="S25" s="5"/>
     </row>
     <row r="26" spans="2:19">
-      <c r="B26" s="15"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
-      <c r="L26" s="11"/>
-      <c r="M26" s="11"/>
-      <c r="N26" s="11"/>
-      <c r="O26" s="11"/>
-      <c r="P26" s="11"/>
-      <c r="Q26" s="11"/>
-      <c r="R26" s="11"/>
+      <c r="B26" s="13"/>
       <c r="S26" s="5"/>
     </row>
     <row r="27" spans="2:19">
-      <c r="B27" s="15"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11"/>
-      <c r="M27" s="11"/>
-      <c r="N27" s="11"/>
-      <c r="O27" s="11"/>
-      <c r="P27" s="11"/>
-      <c r="Q27" s="11"/>
-      <c r="R27" s="11"/>
+      <c r="B27" s="13"/>
       <c r="S27" s="5"/>
     </row>
     <row r="28" spans="2:19">
-      <c r="B28" s="15"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11"/>
-      <c r="L28" s="11"/>
-      <c r="M28" s="11"/>
-      <c r="N28" s="11"/>
-      <c r="O28" s="11"/>
-      <c r="P28" s="11"/>
-      <c r="Q28" s="11"/>
-      <c r="R28" s="11"/>
+      <c r="B28" s="13"/>
       <c r="S28" s="5"/>
     </row>
     <row r="29" spans="2:19">
-      <c r="B29" s="15"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="11"/>
-      <c r="L29" s="11"/>
-      <c r="M29" s="11"/>
-      <c r="N29" s="11"/>
-      <c r="O29" s="11"/>
-      <c r="P29" s="11"/>
-      <c r="Q29" s="11"/>
-      <c r="R29" s="11"/>
+      <c r="B29" s="13"/>
       <c r="S29" s="5"/>
     </row>
     <row r="30" spans="2:19">
-      <c r="B30" s="15"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="11"/>
-      <c r="L30" s="11"/>
-      <c r="M30" s="11"/>
-      <c r="N30" s="11"/>
-      <c r="O30" s="11"/>
-      <c r="P30" s="11"/>
-      <c r="Q30" s="11"/>
-      <c r="R30" s="11"/>
+      <c r="B30" s="13"/>
       <c r="S30" s="5"/>
     </row>
     <row r="31" spans="2:19">
-      <c r="B31" s="15"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11"/>
-      <c r="K31" s="11"/>
-      <c r="L31" s="11"/>
-      <c r="M31" s="11"/>
-      <c r="N31" s="11"/>
-      <c r="O31" s="11"/>
-      <c r="P31" s="11"/>
-      <c r="Q31" s="11"/>
-      <c r="R31" s="11"/>
+      <c r="B31" s="13"/>
       <c r="S31" s="5"/>
     </row>
     <row r="32" spans="2:19">
-      <c r="B32" s="15"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="11"/>
-      <c r="L32" s="11"/>
-      <c r="M32" s="11"/>
-      <c r="N32" s="11"/>
-      <c r="O32" s="11"/>
-      <c r="P32" s="11"/>
-      <c r="Q32" s="11"/>
-      <c r="R32" s="11"/>
+      <c r="B32" s="13"/>
       <c r="S32" s="5"/>
     </row>
     <row r="33" spans="2:19">
-      <c r="B33" s="15"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="11"/>
-      <c r="L33" s="11"/>
-      <c r="M33" s="11"/>
-      <c r="N33" s="11"/>
-      <c r="O33" s="11"/>
-      <c r="P33" s="11"/>
-      <c r="Q33" s="11"/>
-      <c r="R33" s="11"/>
+      <c r="B33" s="13"/>
       <c r="S33" s="5"/>
     </row>
     <row r="34" spans="2:19">
-      <c r="B34" s="15"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="11"/>
-      <c r="L34" s="11"/>
-      <c r="M34" s="11"/>
-      <c r="N34" s="11"/>
-      <c r="O34" s="11"/>
-      <c r="P34" s="11"/>
-      <c r="Q34" s="11"/>
-      <c r="R34" s="11"/>
+      <c r="B34" s="13"/>
       <c r="S34" s="5"/>
     </row>
     <row r="35" spans="2:19">
-      <c r="B35" s="15"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="11"/>
-      <c r="K35" s="11"/>
-      <c r="L35" s="11"/>
-      <c r="M35" s="11"/>
-      <c r="N35" s="11"/>
-      <c r="O35" s="11"/>
-      <c r="P35" s="11"/>
-      <c r="Q35" s="11"/>
-      <c r="R35" s="11"/>
+      <c r="B35" s="13"/>
       <c r="S35" s="5"/>
     </row>
     <row r="36" spans="2:19">
-      <c r="B36" s="15"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="11"/>
-      <c r="K36" s="11"/>
-      <c r="L36" s="11"/>
-      <c r="M36" s="11"/>
-      <c r="N36" s="11"/>
-      <c r="O36" s="11"/>
-      <c r="P36" s="11"/>
-      <c r="Q36" s="11"/>
-      <c r="R36" s="11"/>
+      <c r="B36" s="13"/>
       <c r="S36" s="5"/>
     </row>
     <row r="37" spans="2:19">
-      <c r="B37" s="15"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="11"/>
-      <c r="K37" s="11"/>
-      <c r="L37" s="11"/>
-      <c r="M37" s="11"/>
-      <c r="N37" s="11"/>
-      <c r="O37" s="11"/>
-      <c r="P37" s="11"/>
-      <c r="Q37" s="11"/>
-      <c r="R37" s="11"/>
+      <c r="B37" s="13"/>
       <c r="S37" s="5"/>
     </row>
     <row r="38" spans="2:19">
-      <c r="B38" s="15"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="11"/>
-      <c r="K38" s="11"/>
-      <c r="L38" s="11"/>
-      <c r="M38" s="11"/>
-      <c r="N38" s="11"/>
-      <c r="O38" s="11"/>
-      <c r="P38" s="11"/>
-      <c r="Q38" s="11"/>
-      <c r="R38" s="11"/>
+      <c r="B38" s="13"/>
       <c r="S38" s="5"/>
     </row>
     <row r="39" spans="2:19">
-      <c r="B39" s="15"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="11"/>
-      <c r="K39" s="11"/>
-      <c r="L39" s="11"/>
-      <c r="M39" s="11"/>
-      <c r="N39" s="11"/>
-      <c r="O39" s="11"/>
-      <c r="P39" s="11"/>
-      <c r="Q39" s="11"/>
-      <c r="R39" s="11"/>
+      <c r="B39" s="13"/>
       <c r="S39" s="5"/>
     </row>
     <row r="40" spans="2:19">
-      <c r="B40" s="15"/>
-      <c r="C40" s="11"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
-      <c r="I40" s="11"/>
-      <c r="J40" s="11"/>
-      <c r="K40" s="11"/>
-      <c r="L40" s="11"/>
-      <c r="M40" s="11"/>
-      <c r="N40" s="11"/>
-      <c r="O40" s="11"/>
-      <c r="P40" s="11"/>
-      <c r="Q40" s="11"/>
-      <c r="R40" s="11"/>
+      <c r="B40" s="13"/>
       <c r="S40" s="5"/>
     </row>
     <row r="41" spans="2:19">
-      <c r="B41" s="15"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
-      <c r="I41" s="11"/>
-      <c r="J41" s="11"/>
-      <c r="K41" s="11"/>
-      <c r="L41" s="11"/>
-      <c r="M41" s="11"/>
-      <c r="N41" s="11"/>
-      <c r="O41" s="11"/>
-      <c r="P41" s="11"/>
-      <c r="Q41" s="11"/>
-      <c r="R41" s="11"/>
+      <c r="B41" s="13"/>
       <c r="S41" s="5"/>
     </row>
     <row r="42" spans="2:19">
-      <c r="B42" s="15"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
-      <c r="I42" s="11"/>
-      <c r="J42" s="11"/>
-      <c r="K42" s="11"/>
-      <c r="L42" s="11"/>
-      <c r="M42" s="11"/>
-      <c r="N42" s="11"/>
-      <c r="O42" s="11"/>
-      <c r="P42" s="11"/>
-      <c r="Q42" s="11"/>
-      <c r="R42" s="11"/>
+      <c r="B42" s="13"/>
       <c r="S42" s="5"/>
     </row>
     <row r="43" spans="2:19">
-      <c r="B43" s="15"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="11"/>
-      <c r="H43" s="11"/>
-      <c r="I43" s="11"/>
-      <c r="J43" s="11"/>
-      <c r="K43" s="11"/>
-      <c r="L43" s="11"/>
-      <c r="M43" s="11"/>
-      <c r="N43" s="11"/>
-      <c r="O43" s="11"/>
-      <c r="P43" s="11"/>
-      <c r="Q43" s="11"/>
-      <c r="R43" s="11"/>
+      <c r="B43" s="13"/>
       <c r="S43" s="5"/>
     </row>
     <row r="44" spans="2:19">
-      <c r="B44" s="16"/>
+      <c r="B44" s="14"/>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
@@ -2783,10 +2515,10 @@
       <c r="S44" s="9"/>
     </row>
     <row r="45" spans="2:19">
-      <c r="B45" s="13"/>
+      <c r="B45" s="11"/>
     </row>
     <row r="46" spans="2:19">
-      <c r="B46" s="13"/>
+      <c r="B46" s="11"/>
     </row>
     <row r="47" spans="2:19">
       <c r="B47" t="s">
@@ -2809,124 +2541,71 @@
     </row>
     <row r="49" spans="2:13">
       <c r="B49" s="4"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11"/>
-      <c r="F49" s="11"/>
-      <c r="G49" s="11"/>
-      <c r="H49" s="11"/>
-      <c r="I49" s="11"/>
-      <c r="J49" s="11"/>
       <c r="K49" s="5"/>
     </row>
     <row r="50" spans="2:13">
       <c r="B50" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C50" s="11"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
-      <c r="G50" s="11"/>
-      <c r="H50" s="11"/>
-      <c r="I50" s="11"/>
-      <c r="J50" s="11"/>
       <c r="K50" s="5"/>
     </row>
     <row r="51" spans="2:13">
       <c r="B51" s="4"/>
-      <c r="C51" s="11" t="s">
+      <c r="C51" t="s">
         <v>13</v>
       </c>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11"/>
-      <c r="I51" s="11"/>
-      <c r="J51" s="11"/>
       <c r="K51" s="5"/>
     </row>
     <row r="52" spans="2:13">
       <c r="B52" s="4"/>
-      <c r="C52" s="11"/>
-      <c r="D52" s="12" t="s">
+      <c r="D52" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E52" s="12"/>
-      <c r="F52" s="12"/>
-      <c r="G52" s="11"/>
-      <c r="H52" s="11"/>
-      <c r="I52" s="11"/>
-      <c r="J52" s="11"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
       <c r="K52" s="5"/>
     </row>
     <row r="53" spans="2:13">
       <c r="B53" s="4"/>
-      <c r="C53" s="11"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="12"/>
-      <c r="F53" s="12"/>
-      <c r="G53" s="11"/>
-      <c r="H53" s="11"/>
-      <c r="I53" s="11"/>
-      <c r="J53" s="11"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
       <c r="K53" s="5"/>
     </row>
     <row r="54" spans="2:13">
       <c r="B54" s="4"/>
-      <c r="C54" s="11"/>
-      <c r="D54" s="12" t="s">
+      <c r="D54" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E54" s="12"/>
-      <c r="F54" s="12"/>
-      <c r="G54" s="11"/>
-      <c r="H54" s="11"/>
-      <c r="I54" s="11"/>
-      <c r="J54" s="11"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
       <c r="K54" s="5"/>
     </row>
     <row r="55" spans="2:13">
       <c r="B55" s="4"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="12" t="s">
+      <c r="D55" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E55" s="12"/>
-      <c r="F55" s="12"/>
-      <c r="G55" s="11"/>
-      <c r="H55" s="11"/>
-      <c r="I55" s="11"/>
-      <c r="J55" s="11"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
       <c r="K55" s="5"/>
     </row>
     <row r="56" spans="2:13">
       <c r="B56" s="4"/>
-      <c r="C56" s="11"/>
-      <c r="D56" s="12" t="s">
+      <c r="D56" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E56" s="12"/>
-      <c r="F56" s="12"/>
-      <c r="G56" s="11"/>
-      <c r="H56" s="11"/>
-      <c r="I56" s="11"/>
-      <c r="J56" s="11"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
       <c r="K56" s="5"/>
     </row>
     <row r="57" spans="2:13">
       <c r="B57" s="4"/>
-      <c r="C57" s="11"/>
-      <c r="D57" s="12"/>
-      <c r="E57" s="12" t="s">
+      <c r="D57" s="6"/>
+      <c r="E57" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F57" s="12"/>
-      <c r="G57" s="11"/>
-      <c r="H57" s="11"/>
-      <c r="I57" s="11"/>
-      <c r="J57" s="11"/>
+      <c r="F57" s="6"/>
       <c r="K57" s="5"/>
       <c r="L57" t="s">
         <v>7</v>
@@ -2937,586 +2616,325 @@
     </row>
     <row r="58" spans="2:13">
       <c r="B58" s="4"/>
-      <c r="C58" s="11"/>
-      <c r="D58" s="12" t="s">
+      <c r="D58" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E58" s="12"/>
-      <c r="F58" s="12"/>
-      <c r="G58" s="11"/>
-      <c r="H58" s="11"/>
-      <c r="I58" s="11"/>
-      <c r="J58" s="11"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
       <c r="K58" s="5"/>
     </row>
     <row r="59" spans="2:13">
       <c r="B59" s="4"/>
-      <c r="C59" s="11"/>
-      <c r="D59" s="12" t="s">
+      <c r="D59" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E59" s="12"/>
-      <c r="F59" s="12"/>
-      <c r="G59" s="11"/>
-      <c r="H59" s="11"/>
-      <c r="I59" s="11"/>
-      <c r="J59" s="11"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
       <c r="K59" s="5"/>
     </row>
     <row r="60" spans="2:13">
       <c r="B60" s="4"/>
-      <c r="C60" s="11"/>
-      <c r="D60" s="12" t="s">
+      <c r="D60" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E60" s="12"/>
-      <c r="F60" s="12"/>
-      <c r="G60" s="11"/>
-      <c r="H60" s="11"/>
-      <c r="I60" s="11"/>
-      <c r="J60" s="11"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
       <c r="K60" s="5"/>
     </row>
     <row r="61" spans="2:13">
       <c r="B61" s="4"/>
-      <c r="C61" s="11"/>
-      <c r="D61" s="12" t="s">
+      <c r="D61" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E61" s="12"/>
-      <c r="F61" s="12"/>
-      <c r="G61" s="11"/>
-      <c r="H61" s="11"/>
-      <c r="I61" s="11"/>
-      <c r="J61" s="11"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
       <c r="K61" s="5"/>
     </row>
     <row r="62" spans="2:13">
       <c r="B62" s="4"/>
-      <c r="C62" s="11"/>
-      <c r="D62" s="12" t="s">
+      <c r="D62" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E62" s="12"/>
-      <c r="F62" s="12"/>
-      <c r="G62" s="11"/>
-      <c r="H62" s="11"/>
-      <c r="I62" s="11"/>
-      <c r="J62" s="11"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
       <c r="K62" s="5"/>
     </row>
     <row r="63" spans="2:13">
       <c r="B63" s="4"/>
-      <c r="C63" s="11"/>
-      <c r="D63" s="12" t="s">
+      <c r="D63" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E63" s="12"/>
-      <c r="F63" s="12"/>
-      <c r="G63" s="11"/>
-      <c r="H63" s="11"/>
-      <c r="I63" s="11"/>
-      <c r="J63" s="11"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
       <c r="K63" s="5"/>
     </row>
     <row r="64" spans="2:13">
       <c r="B64" s="4"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="12"/>
-      <c r="E64" s="12" t="s">
+      <c r="D64" s="6"/>
+      <c r="E64" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F64" s="12"/>
-      <c r="G64" s="11"/>
-      <c r="H64" s="11"/>
-      <c r="I64" s="11"/>
-      <c r="J64" s="11"/>
+      <c r="F64" s="6"/>
       <c r="K64" s="5"/>
     </row>
     <row r="65" spans="2:11">
       <c r="B65" s="4"/>
-      <c r="C65" s="11"/>
-      <c r="D65" s="12"/>
-      <c r="E65" s="12" t="s">
+      <c r="D65" s="6"/>
+      <c r="E65" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F65" s="12"/>
-      <c r="G65" s="11"/>
-      <c r="H65" s="11"/>
-      <c r="I65" s="11"/>
-      <c r="J65" s="11"/>
+      <c r="F65" s="6"/>
       <c r="K65" s="5"/>
     </row>
     <row r="66" spans="2:11">
       <c r="B66" s="4"/>
-      <c r="C66" s="11"/>
-      <c r="D66" s="12" t="s">
+      <c r="D66" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E66" s="12"/>
-      <c r="F66" s="12"/>
-      <c r="G66" s="11"/>
-      <c r="H66" s="11"/>
-      <c r="I66" s="11"/>
-      <c r="J66" s="11"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="6"/>
       <c r="K66" s="5"/>
     </row>
     <row r="67" spans="2:11">
       <c r="B67" s="4"/>
-      <c r="C67" s="11"/>
-      <c r="D67" s="12" t="s">
+      <c r="D67" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E67" s="12"/>
-      <c r="F67" s="12"/>
-      <c r="G67" s="11"/>
-      <c r="H67" s="11"/>
-      <c r="I67" s="11"/>
-      <c r="J67" s="11"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="6"/>
       <c r="K67" s="5"/>
     </row>
     <row r="68" spans="2:11">
       <c r="B68" s="4"/>
-      <c r="C68" s="11"/>
-      <c r="D68" s="12" t="s">
+      <c r="D68" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E68" s="12"/>
-      <c r="F68" s="12"/>
-      <c r="G68" s="11"/>
-      <c r="H68" s="11"/>
-      <c r="I68" s="11"/>
-      <c r="J68" s="11"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="6"/>
       <c r="K68" s="5"/>
     </row>
     <row r="69" spans="2:11">
       <c r="B69" s="4"/>
-      <c r="C69" s="11"/>
-      <c r="D69" s="12" t="s">
+      <c r="D69" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E69" s="12"/>
-      <c r="F69" s="12"/>
-      <c r="G69" s="11"/>
-      <c r="H69" s="11"/>
-      <c r="I69" s="11"/>
-      <c r="J69" s="11"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
       <c r="K69" s="5"/>
     </row>
     <row r="70" spans="2:11">
       <c r="B70" s="4"/>
-      <c r="C70" s="11"/>
-      <c r="D70" s="12" t="s">
+      <c r="D70" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E70" s="12"/>
-      <c r="F70" s="12"/>
-      <c r="G70" s="11"/>
-      <c r="H70" s="11"/>
-      <c r="I70" s="11"/>
-      <c r="J70" s="11"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="6"/>
       <c r="K70" s="5"/>
     </row>
     <row r="71" spans="2:11">
       <c r="B71" s="4"/>
-      <c r="C71" s="11"/>
-      <c r="D71" s="12" t="s">
+      <c r="D71" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E71" s="12"/>
-      <c r="F71" s="12"/>
-      <c r="G71" s="11"/>
-      <c r="H71" s="11"/>
-      <c r="I71" s="11"/>
-      <c r="J71" s="11"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
       <c r="K71" s="5"/>
     </row>
     <row r="72" spans="2:11">
       <c r="B72" s="4"/>
-      <c r="C72" s="11"/>
-      <c r="D72" s="12"/>
-      <c r="E72" s="12" t="s">
+      <c r="D72" s="6"/>
+      <c r="E72" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F72" s="12"/>
-      <c r="G72" s="11"/>
-      <c r="H72" s="11"/>
-      <c r="I72" s="11"/>
-      <c r="J72" s="11"/>
+      <c r="F72" s="6"/>
       <c r="K72" s="5"/>
     </row>
     <row r="73" spans="2:11">
       <c r="B73" s="4"/>
-      <c r="C73" s="11"/>
-      <c r="D73" s="12"/>
-      <c r="E73" s="12" t="s">
+      <c r="D73" s="6"/>
+      <c r="E73" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F73" s="12"/>
-      <c r="G73" s="11"/>
-      <c r="H73" s="11"/>
-      <c r="I73" s="11"/>
-      <c r="J73" s="11"/>
+      <c r="F73" s="6"/>
       <c r="K73" s="5"/>
     </row>
     <row r="74" spans="2:11">
       <c r="B74" s="4"/>
-      <c r="C74" s="11"/>
-      <c r="D74" s="12" t="s">
+      <c r="D74" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E74" s="12"/>
-      <c r="F74" s="12"/>
-      <c r="G74" s="11"/>
-      <c r="H74" s="11"/>
-      <c r="I74" s="11"/>
-      <c r="J74" s="11"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
       <c r="K74" s="5"/>
     </row>
     <row r="75" spans="2:11">
       <c r="B75" s="4"/>
-      <c r="C75" s="11"/>
-      <c r="D75" s="12" t="s">
+      <c r="D75" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E75" s="12"/>
-      <c r="F75" s="12"/>
-      <c r="G75" s="11"/>
-      <c r="H75" s="11"/>
-      <c r="I75" s="11"/>
-      <c r="J75" s="11"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
       <c r="K75" s="5"/>
     </row>
     <row r="76" spans="2:11">
       <c r="B76" s="4"/>
-      <c r="C76" s="11" t="s">
+      <c r="C76" t="s">
         <v>17</v>
       </c>
-      <c r="D76" s="11"/>
-      <c r="E76" s="11"/>
-      <c r="F76" s="11"/>
-      <c r="G76" s="11"/>
-      <c r="H76" s="11"/>
-      <c r="I76" s="11"/>
-      <c r="J76" s="11"/>
       <c r="K76" s="5"/>
     </row>
     <row r="77" spans="2:11">
       <c r="B77" s="4"/>
-      <c r="C77" s="11"/>
-      <c r="D77" s="11"/>
-      <c r="E77" s="11"/>
-      <c r="F77" s="11"/>
-      <c r="G77" s="11"/>
-      <c r="H77" s="11"/>
-      <c r="I77" s="11"/>
-      <c r="J77" s="11"/>
       <c r="K77" s="5"/>
     </row>
     <row r="78" spans="2:11">
       <c r="B78" s="4"/>
-      <c r="C78" s="11" t="s">
+      <c r="C78" t="s">
         <v>43</v>
       </c>
-      <c r="D78" s="11"/>
-      <c r="E78" s="11"/>
-      <c r="F78" s="11"/>
-      <c r="G78" s="11"/>
-      <c r="H78" s="11"/>
-      <c r="I78" s="11"/>
-      <c r="J78" s="11"/>
       <c r="K78" s="5"/>
     </row>
     <row r="79" spans="2:11">
       <c r="B79" s="4"/>
-      <c r="C79" s="11" t="s">
+      <c r="C79" t="s">
         <v>44</v>
       </c>
-      <c r="D79" s="11"/>
-      <c r="E79" s="11"/>
-      <c r="F79" s="11"/>
-      <c r="G79" s="11"/>
-      <c r="H79" s="11"/>
-      <c r="I79" s="11"/>
-      <c r="J79" s="11"/>
       <c r="K79" s="5"/>
     </row>
     <row r="80" spans="2:11">
       <c r="B80" s="4"/>
-      <c r="C80" s="11"/>
-      <c r="D80" s="11" t="s">
+      <c r="D80" t="s">
         <v>14</v>
       </c>
-      <c r="E80" s="11"/>
-      <c r="F80" s="11"/>
-      <c r="G80" s="11"/>
-      <c r="H80" s="11"/>
-      <c r="I80" s="11"/>
-      <c r="J80" s="11"/>
       <c r="K80" s="5"/>
     </row>
     <row r="81" spans="2:11">
       <c r="B81" s="4"/>
-      <c r="C81" s="11"/>
-      <c r="D81" s="11" t="s">
+      <c r="D81" t="s">
         <v>15</v>
       </c>
-      <c r="E81" s="11"/>
-      <c r="F81" s="11"/>
-      <c r="G81" s="11"/>
-      <c r="H81" s="11"/>
-      <c r="I81" s="11"/>
-      <c r="J81" s="11"/>
       <c r="K81" s="5"/>
     </row>
     <row r="82" spans="2:11">
       <c r="B82" s="4"/>
-      <c r="C82" s="11"/>
-      <c r="D82" s="11"/>
-      <c r="E82" s="11" t="s">
+      <c r="E82" t="s">
         <v>16</v>
       </c>
-      <c r="F82" s="11"/>
-      <c r="G82" s="11"/>
-      <c r="H82" s="11"/>
-      <c r="I82" s="11"/>
-      <c r="J82" s="11"/>
       <c r="K82" s="5"/>
     </row>
     <row r="83" spans="2:11">
       <c r="B83" s="4"/>
-      <c r="C83" s="11"/>
-      <c r="D83" s="11" t="s">
+      <c r="D83" t="s">
         <v>17</v>
       </c>
-      <c r="E83" s="11"/>
-      <c r="F83" s="11"/>
-      <c r="G83" s="11"/>
-      <c r="H83" s="11"/>
-      <c r="I83" s="11"/>
-      <c r="J83" s="11"/>
       <c r="K83" s="5"/>
     </row>
     <row r="84" spans="2:11">
       <c r="B84" s="4"/>
-      <c r="C84" s="11"/>
-      <c r="D84" s="11"/>
-      <c r="E84" s="11"/>
-      <c r="F84" s="11"/>
-      <c r="G84" s="11"/>
-      <c r="H84" s="11"/>
-      <c r="I84" s="11"/>
-      <c r="J84" s="11"/>
       <c r="K84" s="5"/>
     </row>
     <row r="85" spans="2:11">
       <c r="B85" s="4"/>
-      <c r="C85" s="11"/>
-      <c r="D85" s="11" t="s">
+      <c r="D85" t="s">
         <v>18</v>
       </c>
-      <c r="E85" s="11"/>
-      <c r="F85" s="11"/>
-      <c r="G85" s="11"/>
-      <c r="H85" s="11"/>
-      <c r="I85" s="11"/>
-      <c r="J85" s="11"/>
       <c r="K85" s="5"/>
     </row>
     <row r="86" spans="2:11">
       <c r="B86" s="4"/>
-      <c r="C86" s="11"/>
-      <c r="D86" s="11" t="s">
+      <c r="D86" t="s">
         <v>19</v>
       </c>
-      <c r="E86" s="11"/>
-      <c r="F86" s="11"/>
-      <c r="G86" s="11"/>
-      <c r="H86" s="11"/>
-      <c r="I86" s="11"/>
-      <c r="J86" s="11"/>
       <c r="K86" s="5"/>
     </row>
     <row r="87" spans="2:11">
       <c r="B87" s="4"/>
-      <c r="C87" s="11"/>
-      <c r="D87" s="11" t="s">
+      <c r="D87" t="s">
         <v>20</v>
       </c>
-      <c r="E87" s="11"/>
-      <c r="F87" s="11"/>
-      <c r="G87" s="11"/>
-      <c r="H87" s="11"/>
-      <c r="I87" s="11"/>
-      <c r="J87" s="11"/>
       <c r="K87" s="5"/>
     </row>
     <row r="88" spans="2:11">
       <c r="B88" s="4"/>
-      <c r="C88" s="11"/>
-      <c r="D88" s="11"/>
-      <c r="E88" s="11" t="s">
+      <c r="E88" t="s">
         <v>21</v>
       </c>
-      <c r="F88" s="11"/>
-      <c r="G88" s="11"/>
-      <c r="H88" s="11"/>
-      <c r="I88" s="11"/>
-      <c r="J88" s="11"/>
       <c r="K88" s="5"/>
     </row>
     <row r="89" spans="2:11">
       <c r="B89" s="4"/>
-      <c r="C89" s="11"/>
-      <c r="D89" s="11"/>
-      <c r="E89" s="11" t="s">
+      <c r="E89" t="s">
         <v>22</v>
       </c>
-      <c r="F89" s="11"/>
-      <c r="G89" s="11"/>
-      <c r="H89" s="11"/>
-      <c r="I89" s="11"/>
-      <c r="J89" s="11"/>
       <c r="K89" s="5"/>
     </row>
     <row r="90" spans="2:11">
       <c r="B90" s="4"/>
-      <c r="C90" s="11"/>
-      <c r="D90" s="11" t="s">
+      <c r="D90" t="s">
         <v>17</v>
       </c>
-      <c r="E90" s="11"/>
-      <c r="F90" s="11"/>
-      <c r="G90" s="11"/>
-      <c r="H90" s="11"/>
-      <c r="I90" s="11"/>
-      <c r="J90" s="11"/>
       <c r="K90" s="5"/>
     </row>
     <row r="91" spans="2:11">
       <c r="B91" s="4"/>
-      <c r="C91" s="11"/>
-      <c r="D91" s="11"/>
-      <c r="E91" s="11"/>
-      <c r="F91" s="11"/>
-      <c r="G91" s="11"/>
-      <c r="H91" s="11"/>
-      <c r="I91" s="11"/>
-      <c r="J91" s="11"/>
       <c r="K91" s="5"/>
     </row>
     <row r="92" spans="2:11">
       <c r="B92" s="4"/>
-      <c r="C92" s="11"/>
-      <c r="D92" s="11" t="s">
+      <c r="D92" t="s">
         <v>23</v>
       </c>
-      <c r="E92" s="11"/>
-      <c r="F92" s="11"/>
-      <c r="G92" s="11"/>
-      <c r="H92" s="11"/>
-      <c r="I92" s="11"/>
-      <c r="J92" s="11"/>
       <c r="K92" s="5"/>
     </row>
     <row r="93" spans="2:11">
       <c r="B93" s="4"/>
-      <c r="C93" s="11"/>
-      <c r="D93" s="11" t="s">
+      <c r="D93" t="s">
         <v>24</v>
       </c>
-      <c r="E93" s="11"/>
-      <c r="F93" s="11"/>
-      <c r="G93" s="11"/>
-      <c r="H93" s="11"/>
-      <c r="I93" s="11"/>
-      <c r="J93" s="11"/>
       <c r="K93" s="5"/>
     </row>
     <row r="94" spans="2:11">
       <c r="B94" s="4"/>
-      <c r="C94" s="11"/>
-      <c r="D94" s="11" t="s">
+      <c r="D94" t="s">
         <v>25</v>
       </c>
-      <c r="E94" s="11"/>
-      <c r="F94" s="11"/>
-      <c r="G94" s="11"/>
-      <c r="H94" s="11"/>
-      <c r="I94" s="11"/>
-      <c r="J94" s="11"/>
       <c r="K94" s="5"/>
     </row>
     <row r="95" spans="2:11">
       <c r="B95" s="4"/>
-      <c r="C95" s="11"/>
-      <c r="D95" s="11"/>
-      <c r="E95" s="11" t="s">
+      <c r="E95" t="s">
         <v>26</v>
       </c>
-      <c r="F95" s="11"/>
-      <c r="G95" s="11"/>
-      <c r="H95" s="11"/>
-      <c r="I95" s="11"/>
-      <c r="J95" s="11"/>
       <c r="K95" s="5"/>
     </row>
     <row r="96" spans="2:11">
       <c r="B96" s="4"/>
-      <c r="C96" s="11"/>
-      <c r="D96" s="11"/>
-      <c r="E96" s="11" t="s">
+      <c r="E96" t="s">
         <v>27</v>
       </c>
-      <c r="F96" s="11" t="s">
+      <c r="F96" t="s">
         <v>28</v>
       </c>
-      <c r="G96" s="11"/>
-      <c r="H96" s="11"/>
-      <c r="I96" s="11"/>
-      <c r="J96" s="11"/>
       <c r="K96" s="5"/>
     </row>
     <row r="97" spans="2:11">
       <c r="B97" s="4"/>
-      <c r="C97" s="11"/>
-      <c r="D97" s="11" t="s">
+      <c r="D97" t="s">
         <v>29</v>
       </c>
-      <c r="E97" s="11"/>
-      <c r="F97" s="11"/>
-      <c r="G97" s="11"/>
-      <c r="H97" s="11"/>
-      <c r="I97" s="11"/>
-      <c r="J97" s="11"/>
       <c r="K97" s="5"/>
     </row>
     <row r="98" spans="2:11">
       <c r="B98" s="4"/>
-      <c r="C98" s="11" t="s">
+      <c r="C98" t="s">
         <v>17</v>
       </c>
-      <c r="D98" s="11"/>
-      <c r="E98" s="11"/>
-      <c r="F98" s="11"/>
-      <c r="G98" s="11"/>
-      <c r="H98" s="11"/>
-      <c r="I98" s="11"/>
-      <c r="J98" s="11"/>
       <c r="K98" s="5"/>
     </row>
     <row r="99" spans="2:11">
       <c r="B99" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C99" s="11"/>
-      <c r="D99" s="11"/>
-      <c r="E99" s="11"/>
-      <c r="F99" s="11"/>
-      <c r="G99" s="11"/>
-      <c r="H99" s="11"/>
-      <c r="I99" s="11"/>
-      <c r="J99" s="11"/>
       <c r="K99" s="5"/>
     </row>
     <row r="100" spans="2:11">
@@ -3549,436 +2967,126 @@
     </row>
     <row r="138" spans="2:13">
       <c r="B138" s="4"/>
-      <c r="C138" s="11"/>
-      <c r="D138" s="11"/>
-      <c r="E138" s="11"/>
-      <c r="F138" s="11"/>
-      <c r="G138" s="11"/>
-      <c r="H138" s="11"/>
-      <c r="I138" s="11"/>
-      <c r="J138" s="11"/>
-      <c r="K138" s="11"/>
-      <c r="L138" s="11"/>
       <c r="M138" s="5"/>
     </row>
     <row r="139" spans="2:13">
       <c r="B139" s="4"/>
-      <c r="C139" s="11"/>
-      <c r="D139" s="11"/>
-      <c r="E139" s="11"/>
-      <c r="F139" s="11"/>
-      <c r="G139" s="11"/>
-      <c r="H139" s="11"/>
-      <c r="I139" s="11"/>
-      <c r="J139" s="11"/>
-      <c r="K139" s="11"/>
-      <c r="L139" s="11"/>
       <c r="M139" s="5"/>
     </row>
     <row r="140" spans="2:13">
       <c r="B140" s="4"/>
-      <c r="C140" s="11"/>
-      <c r="D140" s="11"/>
-      <c r="E140" s="11"/>
-      <c r="F140" s="11"/>
-      <c r="G140" s="11"/>
-      <c r="H140" s="11"/>
-      <c r="I140" s="11"/>
-      <c r="J140" s="11"/>
-      <c r="K140" s="11"/>
-      <c r="L140" s="11"/>
       <c r="M140" s="5"/>
     </row>
     <row r="141" spans="2:13">
       <c r="B141" s="4"/>
-      <c r="C141" s="11"/>
-      <c r="D141" s="11"/>
-      <c r="E141" s="11"/>
-      <c r="F141" s="11"/>
-      <c r="G141" s="11"/>
-      <c r="H141" s="11"/>
-      <c r="I141" s="11"/>
-      <c r="J141" s="11"/>
-      <c r="K141" s="11"/>
-      <c r="L141" s="11"/>
       <c r="M141" s="5"/>
     </row>
     <row r="142" spans="2:13">
       <c r="B142" s="4"/>
-      <c r="C142" s="11"/>
-      <c r="D142" s="11"/>
-      <c r="E142" s="11"/>
-      <c r="F142" s="11"/>
-      <c r="G142" s="11"/>
-      <c r="H142" s="11"/>
-      <c r="I142" s="11"/>
-      <c r="J142" s="11"/>
-      <c r="K142" s="11"/>
-      <c r="L142" s="11"/>
       <c r="M142" s="5"/>
     </row>
     <row r="143" spans="2:13">
       <c r="B143" s="4"/>
-      <c r="C143" s="11"/>
-      <c r="D143" s="11"/>
-      <c r="E143" s="11"/>
-      <c r="F143" s="11"/>
-      <c r="G143" s="11"/>
-      <c r="H143" s="11"/>
-      <c r="I143" s="11"/>
-      <c r="J143" s="11"/>
-      <c r="K143" s="11"/>
-      <c r="L143" s="11"/>
       <c r="M143" s="5"/>
     </row>
     <row r="144" spans="2:13">
       <c r="B144" s="4"/>
-      <c r="C144" s="11"/>
-      <c r="D144" s="11"/>
-      <c r="E144" s="11"/>
-      <c r="F144" s="11"/>
-      <c r="G144" s="11"/>
-      <c r="H144" s="11"/>
-      <c r="I144" s="11"/>
-      <c r="J144" s="11"/>
-      <c r="K144" s="11"/>
-      <c r="L144" s="11"/>
       <c r="M144" s="5"/>
     </row>
     <row r="145" spans="2:13">
       <c r="B145" s="4"/>
-      <c r="C145" s="11"/>
-      <c r="D145" s="11"/>
-      <c r="E145" s="11"/>
-      <c r="F145" s="11"/>
-      <c r="G145" s="11"/>
-      <c r="H145" s="11"/>
-      <c r="I145" s="11"/>
-      <c r="J145" s="11"/>
-      <c r="K145" s="11"/>
-      <c r="L145" s="11"/>
       <c r="M145" s="5"/>
     </row>
     <row r="146" spans="2:13">
       <c r="B146" s="4"/>
-      <c r="C146" s="11"/>
-      <c r="D146" s="11"/>
-      <c r="E146" s="11"/>
-      <c r="F146" s="11"/>
-      <c r="G146" s="11"/>
-      <c r="H146" s="11"/>
-      <c r="I146" s="11"/>
-      <c r="J146" s="11"/>
-      <c r="K146" s="11"/>
-      <c r="L146" s="11"/>
       <c r="M146" s="5"/>
     </row>
     <row r="147" spans="2:13">
       <c r="B147" s="4"/>
-      <c r="C147" s="11"/>
-      <c r="D147" s="11"/>
-      <c r="E147" s="11"/>
-      <c r="F147" s="11"/>
-      <c r="G147" s="11"/>
-      <c r="H147" s="11"/>
-      <c r="I147" s="11"/>
-      <c r="J147" s="11"/>
-      <c r="K147" s="11"/>
-      <c r="L147" s="11"/>
       <c r="M147" s="5"/>
     </row>
     <row r="148" spans="2:13">
       <c r="B148" s="4"/>
-      <c r="C148" s="11"/>
-      <c r="D148" s="11"/>
-      <c r="E148" s="11"/>
-      <c r="F148" s="11"/>
-      <c r="G148" s="11"/>
-      <c r="H148" s="11"/>
-      <c r="I148" s="11"/>
-      <c r="J148" s="11"/>
-      <c r="K148" s="11"/>
-      <c r="L148" s="11"/>
       <c r="M148" s="5"/>
     </row>
     <row r="149" spans="2:13">
       <c r="B149" s="4"/>
-      <c r="C149" s="11"/>
-      <c r="D149" s="11"/>
-      <c r="E149" s="11"/>
-      <c r="F149" s="11"/>
-      <c r="G149" s="11"/>
-      <c r="H149" s="11"/>
-      <c r="I149" s="11"/>
-      <c r="J149" s="11"/>
-      <c r="K149" s="11"/>
-      <c r="L149" s="11"/>
       <c r="M149" s="5"/>
     </row>
     <row r="150" spans="2:13">
       <c r="B150" s="4"/>
-      <c r="C150" s="11"/>
-      <c r="D150" s="11"/>
-      <c r="E150" s="11"/>
-      <c r="F150" s="11"/>
-      <c r="G150" s="11"/>
-      <c r="H150" s="11"/>
-      <c r="I150" s="11"/>
-      <c r="J150" s="11"/>
-      <c r="K150" s="11"/>
-      <c r="L150" s="11"/>
       <c r="M150" s="5"/>
     </row>
     <row r="151" spans="2:13">
       <c r="B151" s="4"/>
-      <c r="C151" s="11"/>
-      <c r="D151" s="11"/>
-      <c r="E151" s="11"/>
-      <c r="F151" s="11"/>
-      <c r="G151" s="11"/>
-      <c r="H151" s="11"/>
-      <c r="I151" s="11"/>
-      <c r="J151" s="11"/>
-      <c r="K151" s="11"/>
-      <c r="L151" s="11"/>
       <c r="M151" s="5"/>
     </row>
     <row r="152" spans="2:13">
       <c r="B152" s="4"/>
-      <c r="C152" s="11"/>
-      <c r="D152" s="11"/>
-      <c r="E152" s="11"/>
-      <c r="F152" s="11"/>
-      <c r="G152" s="11"/>
-      <c r="H152" s="11"/>
-      <c r="I152" s="11"/>
-      <c r="J152" s="11"/>
-      <c r="K152" s="11"/>
-      <c r="L152" s="11"/>
       <c r="M152" s="5"/>
     </row>
     <row r="153" spans="2:13">
       <c r="B153" s="4"/>
-      <c r="C153" s="11"/>
-      <c r="D153" s="11"/>
-      <c r="E153" s="11"/>
-      <c r="F153" s="11"/>
-      <c r="G153" s="11"/>
-      <c r="H153" s="11"/>
-      <c r="I153" s="11"/>
-      <c r="J153" s="11"/>
-      <c r="K153" s="11"/>
-      <c r="L153" s="11"/>
       <c r="M153" s="5"/>
     </row>
     <row r="154" spans="2:13">
       <c r="B154" s="4"/>
-      <c r="C154" s="11"/>
-      <c r="D154" s="11"/>
-      <c r="E154" s="11"/>
-      <c r="F154" s="11"/>
-      <c r="G154" s="11"/>
-      <c r="H154" s="11"/>
-      <c r="I154" s="11"/>
-      <c r="J154" s="11"/>
-      <c r="K154" s="11"/>
-      <c r="L154" s="11"/>
       <c r="M154" s="5"/>
     </row>
     <row r="155" spans="2:13">
       <c r="B155" s="4"/>
-      <c r="C155" s="11"/>
-      <c r="D155" s="11"/>
-      <c r="E155" s="11"/>
-      <c r="F155" s="11"/>
-      <c r="G155" s="11"/>
-      <c r="H155" s="11"/>
-      <c r="I155" s="11"/>
-      <c r="J155" s="11"/>
-      <c r="K155" s="11"/>
-      <c r="L155" s="11"/>
       <c r="M155" s="5"/>
     </row>
     <row r="156" spans="2:13">
       <c r="B156" s="4"/>
-      <c r="C156" s="11"/>
-      <c r="D156" s="11"/>
-      <c r="E156" s="11"/>
-      <c r="F156" s="11"/>
-      <c r="G156" s="11"/>
-      <c r="H156" s="11"/>
-      <c r="I156" s="11"/>
-      <c r="J156" s="11"/>
-      <c r="K156" s="11"/>
-      <c r="L156" s="11"/>
       <c r="M156" s="5"/>
     </row>
     <row r="157" spans="2:13">
       <c r="B157" s="4"/>
-      <c r="C157" s="11"/>
-      <c r="D157" s="11"/>
-      <c r="E157" s="11"/>
-      <c r="F157" s="11"/>
-      <c r="G157" s="11"/>
-      <c r="H157" s="11"/>
-      <c r="I157" s="11"/>
-      <c r="J157" s="11"/>
-      <c r="K157" s="11"/>
-      <c r="L157" s="11"/>
       <c r="M157" s="5"/>
     </row>
     <row r="158" spans="2:13">
       <c r="B158" s="4"/>
-      <c r="C158" s="11"/>
-      <c r="D158" s="11"/>
-      <c r="E158" s="11"/>
-      <c r="F158" s="11"/>
-      <c r="G158" s="11"/>
-      <c r="H158" s="11"/>
-      <c r="I158" s="11"/>
-      <c r="J158" s="11"/>
-      <c r="K158" s="11"/>
-      <c r="L158" s="11"/>
       <c r="M158" s="5"/>
     </row>
     <row r="159" spans="2:13">
       <c r="B159" s="4"/>
-      <c r="C159" s="11"/>
-      <c r="D159" s="11"/>
-      <c r="E159" s="11"/>
-      <c r="F159" s="11"/>
-      <c r="G159" s="11"/>
-      <c r="H159" s="11"/>
-      <c r="I159" s="11"/>
-      <c r="J159" s="11"/>
-      <c r="K159" s="11"/>
-      <c r="L159" s="11"/>
       <c r="M159" s="5"/>
     </row>
     <row r="160" spans="2:13">
       <c r="B160" s="4"/>
-      <c r="C160" s="11"/>
-      <c r="D160" s="11"/>
-      <c r="E160" s="11"/>
-      <c r="F160" s="11"/>
-      <c r="G160" s="11"/>
-      <c r="H160" s="11"/>
-      <c r="I160" s="11"/>
-      <c r="J160" s="11"/>
-      <c r="K160" s="11"/>
-      <c r="L160" s="11"/>
       <c r="M160" s="5"/>
     </row>
     <row r="161" spans="2:13">
       <c r="B161" s="4"/>
-      <c r="C161" s="11"/>
-      <c r="D161" s="11"/>
-      <c r="E161" s="11"/>
-      <c r="F161" s="11"/>
-      <c r="G161" s="11"/>
-      <c r="H161" s="11"/>
-      <c r="I161" s="11"/>
-      <c r="J161" s="11"/>
-      <c r="K161" s="11"/>
-      <c r="L161" s="11"/>
       <c r="M161" s="5"/>
     </row>
     <row r="162" spans="2:13">
       <c r="B162" s="4"/>
-      <c r="C162" s="11"/>
-      <c r="D162" s="11"/>
-      <c r="E162" s="11"/>
-      <c r="F162" s="11"/>
-      <c r="G162" s="11"/>
-      <c r="H162" s="11"/>
-      <c r="I162" s="11"/>
-      <c r="J162" s="11"/>
-      <c r="K162" s="11"/>
-      <c r="L162" s="11"/>
       <c r="M162" s="5"/>
     </row>
     <row r="163" spans="2:13">
       <c r="B163" s="4"/>
-      <c r="C163" s="11"/>
-      <c r="D163" s="11"/>
-      <c r="E163" s="11"/>
-      <c r="F163" s="11"/>
-      <c r="G163" s="11"/>
-      <c r="H163" s="11"/>
-      <c r="I163" s="11"/>
-      <c r="J163" s="11"/>
-      <c r="K163" s="11"/>
-      <c r="L163" s="11"/>
       <c r="M163" s="5"/>
     </row>
     <row r="164" spans="2:13">
       <c r="B164" s="4"/>
-      <c r="C164" s="11"/>
-      <c r="D164" s="11"/>
-      <c r="E164" s="11"/>
-      <c r="F164" s="11"/>
-      <c r="G164" s="11"/>
-      <c r="H164" s="11"/>
-      <c r="I164" s="11"/>
-      <c r="J164" s="11"/>
-      <c r="K164" s="11"/>
-      <c r="L164" s="11"/>
       <c r="M164" s="5"/>
     </row>
     <row r="165" spans="2:13">
       <c r="B165" s="4"/>
-      <c r="C165" s="11"/>
-      <c r="D165" s="11"/>
-      <c r="E165" s="11"/>
-      <c r="F165" s="11"/>
-      <c r="G165" s="11"/>
-      <c r="H165" s="11"/>
-      <c r="I165" s="11"/>
-      <c r="J165" s="11"/>
-      <c r="K165" s="11"/>
-      <c r="L165" s="11"/>
       <c r="M165" s="5"/>
     </row>
     <row r="166" spans="2:13">
       <c r="B166" s="4"/>
-      <c r="C166" s="11"/>
-      <c r="D166" s="11"/>
-      <c r="E166" s="11"/>
-      <c r="F166" s="11"/>
-      <c r="G166" s="11"/>
-      <c r="H166" s="11"/>
-      <c r="I166" s="11"/>
-      <c r="J166" s="11"/>
-      <c r="K166" s="11"/>
-      <c r="L166" s="11"/>
       <c r="M166" s="5"/>
     </row>
     <row r="167" spans="2:13">
       <c r="B167" s="4"/>
-      <c r="C167" s="11"/>
-      <c r="D167" s="11"/>
-      <c r="E167" s="11"/>
-      <c r="F167" s="11"/>
-      <c r="G167" s="11"/>
-      <c r="H167" s="11"/>
-      <c r="I167" s="11"/>
-      <c r="J167" s="11"/>
-      <c r="K167" s="11"/>
-      <c r="L167" s="11"/>
       <c r="M167" s="5"/>
     </row>
     <row r="168" spans="2:13">
       <c r="B168" s="4"/>
-      <c r="C168" s="11"/>
-      <c r="D168" s="11"/>
-      <c r="E168" s="11"/>
-      <c r="F168" s="11"/>
-      <c r="G168" s="11"/>
-      <c r="H168" s="11"/>
-      <c r="I168" s="11"/>
-      <c r="J168" s="11"/>
-      <c r="K168" s="11"/>
-      <c r="L168" s="11"/>
       <c r="M168" s="5"/>
     </row>
     <row r="169" spans="2:13">
@@ -4000,4 +3108,1579 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AEFE6AB-3E4D-4AFC-855A-253B49BCCDA1}">
+  <dimension ref="B3:N150"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="P28" sqref="P28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetData>
+    <row r="3" spans="2:12">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="2:12">
+      <c r="B4" s="4"/>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="2:12">
+      <c r="B5" s="4"/>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="2:12">
+      <c r="B6" s="4"/>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="2:12">
+      <c r="B7" s="4"/>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="2:12">
+      <c r="B8" s="4"/>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="2:12">
+      <c r="B9" s="4"/>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="2:12">
+      <c r="B10" s="4"/>
+      <c r="E10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12">
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="9"/>
+    </row>
+    <row r="14" spans="2:12">
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12">
+      <c r="B15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" spans="2:12">
+      <c r="B16" s="4"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="5"/>
+    </row>
+    <row r="17" spans="2:14">
+      <c r="B17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="5"/>
+    </row>
+    <row r="18" spans="2:14">
+      <c r="B18" s="4"/>
+      <c r="C18" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="5"/>
+    </row>
+    <row r="19" spans="2:14">
+      <c r="B19" s="4"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="17"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="5"/>
+    </row>
+    <row r="20" spans="2:14">
+      <c r="B20" s="4"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="17"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="5"/>
+    </row>
+    <row r="21" spans="2:14">
+      <c r="B21" s="4"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="5"/>
+    </row>
+    <row r="22" spans="2:14">
+      <c r="B22" s="4"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="5"/>
+    </row>
+    <row r="23" spans="2:14">
+      <c r="B23" s="4"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="5"/>
+    </row>
+    <row r="24" spans="2:14">
+      <c r="B24" s="4"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="5"/>
+    </row>
+    <row r="25" spans="2:14">
+      <c r="B25" s="4"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="5"/>
+      <c r="M25" t="s">
+        <v>7</v>
+      </c>
+      <c r="N25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14">
+      <c r="B26" s="4"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="5"/>
+    </row>
+    <row r="27" spans="2:14">
+      <c r="B27" s="4"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="17"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="5"/>
+    </row>
+    <row r="28" spans="2:14">
+      <c r="B28" s="4"/>
+      <c r="C28" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="5"/>
+    </row>
+    <row r="29" spans="2:14">
+      <c r="B29" s="4"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="15"/>
+      <c r="L29" s="5"/>
+    </row>
+    <row r="30" spans="2:14">
+      <c r="B30" s="4"/>
+      <c r="C30" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="5"/>
+    </row>
+    <row r="31" spans="2:14">
+      <c r="B31" s="4"/>
+      <c r="C31" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="5"/>
+    </row>
+    <row r="32" spans="2:14">
+      <c r="B32" s="4"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="5"/>
+    </row>
+    <row r="33" spans="2:12">
+      <c r="B33" s="4"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="5"/>
+    </row>
+    <row r="34" spans="2:12">
+      <c r="B34" s="4"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="5"/>
+    </row>
+    <row r="35" spans="2:12">
+      <c r="B35" s="4"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="5"/>
+    </row>
+    <row r="36" spans="2:12">
+      <c r="B36" s="4"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
+      <c r="K36" s="15"/>
+      <c r="L36" s="5"/>
+    </row>
+    <row r="37" spans="2:12">
+      <c r="B37" s="4"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="15"/>
+      <c r="L37" s="5"/>
+    </row>
+    <row r="38" spans="2:12">
+      <c r="B38" s="4"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="15"/>
+      <c r="K38" s="15"/>
+      <c r="L38" s="5"/>
+    </row>
+    <row r="39" spans="2:12">
+      <c r="B39" s="4"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="15"/>
+      <c r="J39" s="15"/>
+      <c r="K39" s="15"/>
+      <c r="L39" s="5"/>
+    </row>
+    <row r="40" spans="2:12">
+      <c r="B40" s="4"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="15"/>
+      <c r="K40" s="15"/>
+      <c r="L40" s="5"/>
+    </row>
+    <row r="41" spans="2:12">
+      <c r="B41" s="4"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="15"/>
+      <c r="J41" s="15"/>
+      <c r="K41" s="15"/>
+      <c r="L41" s="5"/>
+    </row>
+    <row r="42" spans="2:12">
+      <c r="B42" s="4"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="15"/>
+      <c r="J42" s="15"/>
+      <c r="K42" s="15"/>
+      <c r="L42" s="5"/>
+    </row>
+    <row r="43" spans="2:12">
+      <c r="B43" s="4"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="15"/>
+      <c r="J43" s="15"/>
+      <c r="K43" s="15"/>
+      <c r="L43" s="5"/>
+    </row>
+    <row r="44" spans="2:12">
+      <c r="B44" s="4"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="15"/>
+      <c r="J44" s="15"/>
+      <c r="K44" s="15"/>
+      <c r="L44" s="5"/>
+    </row>
+    <row r="45" spans="2:12">
+      <c r="B45" s="4"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="15"/>
+      <c r="J45" s="15"/>
+      <c r="K45" s="15"/>
+      <c r="L45" s="5"/>
+    </row>
+    <row r="46" spans="2:12">
+      <c r="B46" s="4"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="15"/>
+      <c r="I46" s="15"/>
+      <c r="J46" s="15"/>
+      <c r="K46" s="15"/>
+      <c r="L46" s="5"/>
+    </row>
+    <row r="47" spans="2:12">
+      <c r="B47" s="4"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E47" s="15"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="15"/>
+      <c r="J47" s="15"/>
+      <c r="K47" s="15"/>
+      <c r="L47" s="5"/>
+    </row>
+    <row r="48" spans="2:12">
+      <c r="B48" s="4"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E48" s="15"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="15"/>
+      <c r="H48" s="15"/>
+      <c r="I48" s="15"/>
+      <c r="J48" s="15"/>
+      <c r="K48" s="15"/>
+      <c r="L48" s="5"/>
+    </row>
+    <row r="49" spans="2:12">
+      <c r="B49" s="4"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E49" s="15"/>
+      <c r="F49" s="15"/>
+      <c r="G49" s="15"/>
+      <c r="H49" s="15"/>
+      <c r="I49" s="15"/>
+      <c r="J49" s="15"/>
+      <c r="K49" s="15"/>
+      <c r="L49" s="5"/>
+    </row>
+    <row r="50" spans="2:12">
+      <c r="B50" s="4"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E50" s="15"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="15"/>
+      <c r="H50" s="15"/>
+      <c r="I50" s="15"/>
+      <c r="J50" s="15"/>
+      <c r="K50" s="15"/>
+      <c r="L50" s="5"/>
+    </row>
+    <row r="51" spans="2:12">
+      <c r="B51" s="4"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E51" s="15"/>
+      <c r="F51" s="15"/>
+      <c r="G51" s="15"/>
+      <c r="H51" s="15"/>
+      <c r="I51" s="15"/>
+      <c r="J51" s="15"/>
+      <c r="K51" s="15"/>
+      <c r="L51" s="5"/>
+    </row>
+    <row r="52" spans="2:12">
+      <c r="B52" s="4"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F52" s="15"/>
+      <c r="G52" s="15"/>
+      <c r="H52" s="15"/>
+      <c r="I52" s="15"/>
+      <c r="J52" s="15"/>
+      <c r="K52" s="15"/>
+      <c r="L52" s="5"/>
+    </row>
+    <row r="53" spans="2:12">
+      <c r="B53" s="4"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F53" s="15"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="15"/>
+      <c r="I53" s="15"/>
+      <c r="J53" s="15"/>
+      <c r="K53" s="15"/>
+      <c r="L53" s="5"/>
+    </row>
+    <row r="54" spans="2:12">
+      <c r="B54" s="4"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E54" s="15"/>
+      <c r="F54" s="15"/>
+      <c r="G54" s="15"/>
+      <c r="H54" s="15"/>
+      <c r="I54" s="15"/>
+      <c r="J54" s="15"/>
+      <c r="K54" s="15"/>
+      <c r="L54" s="5"/>
+    </row>
+    <row r="55" spans="2:12">
+      <c r="B55" s="4"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="15"/>
+      <c r="I55" s="15"/>
+      <c r="J55" s="15"/>
+      <c r="K55" s="15"/>
+      <c r="L55" s="5"/>
+    </row>
+    <row r="56" spans="2:12">
+      <c r="B56" s="4"/>
+      <c r="C56" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D56" s="15"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="15"/>
+      <c r="G56" s="15"/>
+      <c r="H56" s="15"/>
+      <c r="I56" s="15"/>
+      <c r="J56" s="15"/>
+      <c r="K56" s="15"/>
+      <c r="L56" s="5"/>
+    </row>
+    <row r="57" spans="2:12">
+      <c r="B57" s="4"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="15"/>
+      <c r="G57" s="15"/>
+      <c r="H57" s="15"/>
+      <c r="I57" s="15"/>
+      <c r="J57" s="15"/>
+      <c r="K57" s="15"/>
+      <c r="L57" s="5"/>
+    </row>
+    <row r="58" spans="2:12">
+      <c r="B58" s="4"/>
+      <c r="C58" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D58" s="15"/>
+      <c r="E58" s="15"/>
+      <c r="F58" s="15"/>
+      <c r="G58" s="15"/>
+      <c r="H58" s="15"/>
+      <c r="I58" s="15"/>
+      <c r="J58" s="15"/>
+      <c r="K58" s="15"/>
+      <c r="L58" s="5"/>
+    </row>
+    <row r="59" spans="2:12">
+      <c r="B59" s="4"/>
+      <c r="C59" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D59" s="15"/>
+      <c r="E59" s="15"/>
+      <c r="F59" s="15"/>
+      <c r="G59" s="15"/>
+      <c r="H59" s="15"/>
+      <c r="I59" s="15"/>
+      <c r="J59" s="15"/>
+      <c r="K59" s="15"/>
+      <c r="L59" s="5"/>
+    </row>
+    <row r="60" spans="2:12">
+      <c r="B60" s="4"/>
+      <c r="C60" s="15"/>
+      <c r="D60" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E60" s="15"/>
+      <c r="F60" s="15"/>
+      <c r="G60" s="15"/>
+      <c r="H60" s="15"/>
+      <c r="I60" s="15"/>
+      <c r="J60" s="15"/>
+      <c r="K60" s="15"/>
+      <c r="L60" s="5"/>
+    </row>
+    <row r="61" spans="2:12">
+      <c r="B61" s="4"/>
+      <c r="C61" s="15"/>
+      <c r="D61" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E61" s="15"/>
+      <c r="F61" s="15"/>
+      <c r="G61" s="15"/>
+      <c r="H61" s="15"/>
+      <c r="I61" s="15"/>
+      <c r="J61" s="15"/>
+      <c r="K61" s="15"/>
+      <c r="L61" s="5"/>
+    </row>
+    <row r="62" spans="2:12">
+      <c r="B62" s="4"/>
+      <c r="C62" s="15"/>
+      <c r="D62" s="15"/>
+      <c r="E62" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F62" s="15"/>
+      <c r="G62" s="15"/>
+      <c r="H62" s="15"/>
+      <c r="I62" s="15"/>
+      <c r="J62" s="15"/>
+      <c r="K62" s="15"/>
+      <c r="L62" s="5"/>
+    </row>
+    <row r="63" spans="2:12">
+      <c r="B63" s="4"/>
+      <c r="C63" s="15"/>
+      <c r="D63" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E63" s="15"/>
+      <c r="F63" s="15"/>
+      <c r="G63" s="15"/>
+      <c r="H63" s="15"/>
+      <c r="I63" s="15"/>
+      <c r="J63" s="15"/>
+      <c r="K63" s="15"/>
+      <c r="L63" s="5"/>
+    </row>
+    <row r="64" spans="2:12">
+      <c r="B64" s="4"/>
+      <c r="C64" s="15"/>
+      <c r="D64" s="15"/>
+      <c r="E64" s="15"/>
+      <c r="F64" s="15"/>
+      <c r="G64" s="15"/>
+      <c r="H64" s="15"/>
+      <c r="I64" s="15"/>
+      <c r="J64" s="15"/>
+      <c r="K64" s="15"/>
+      <c r="L64" s="5"/>
+    </row>
+    <row r="65" spans="2:12">
+      <c r="B65" s="4"/>
+      <c r="C65" s="15"/>
+      <c r="D65" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E65" s="15"/>
+      <c r="F65" s="15"/>
+      <c r="G65" s="15"/>
+      <c r="H65" s="15"/>
+      <c r="I65" s="15"/>
+      <c r="J65" s="15"/>
+      <c r="K65" s="15"/>
+      <c r="L65" s="5"/>
+    </row>
+    <row r="66" spans="2:12">
+      <c r="B66" s="4"/>
+      <c r="C66" s="15"/>
+      <c r="D66" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E66" s="15"/>
+      <c r="F66" s="15"/>
+      <c r="G66" s="15"/>
+      <c r="H66" s="15"/>
+      <c r="I66" s="15"/>
+      <c r="J66" s="15"/>
+      <c r="K66" s="15"/>
+      <c r="L66" s="5"/>
+    </row>
+    <row r="67" spans="2:12">
+      <c r="B67" s="4"/>
+      <c r="C67" s="15"/>
+      <c r="D67" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E67" s="15"/>
+      <c r="F67" s="15"/>
+      <c r="G67" s="15"/>
+      <c r="H67" s="15"/>
+      <c r="I67" s="15"/>
+      <c r="J67" s="15"/>
+      <c r="K67" s="15"/>
+      <c r="L67" s="5"/>
+    </row>
+    <row r="68" spans="2:12">
+      <c r="B68" s="4"/>
+      <c r="C68" s="15"/>
+      <c r="D68" s="15"/>
+      <c r="E68" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F68" s="15"/>
+      <c r="G68" s="15"/>
+      <c r="H68" s="15"/>
+      <c r="I68" s="15"/>
+      <c r="J68" s="15"/>
+      <c r="K68" s="15"/>
+      <c r="L68" s="5"/>
+    </row>
+    <row r="69" spans="2:12">
+      <c r="B69" s="4"/>
+      <c r="C69" s="15"/>
+      <c r="D69" s="15"/>
+      <c r="E69" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F69" s="15"/>
+      <c r="G69" s="15"/>
+      <c r="H69" s="15"/>
+      <c r="I69" s="15"/>
+      <c r="J69" s="15"/>
+      <c r="K69" s="15"/>
+      <c r="L69" s="5"/>
+    </row>
+    <row r="70" spans="2:12">
+      <c r="B70" s="4"/>
+      <c r="C70" s="15"/>
+      <c r="D70" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E70" s="15"/>
+      <c r="F70" s="15"/>
+      <c r="G70" s="15"/>
+      <c r="H70" s="15"/>
+      <c r="I70" s="15"/>
+      <c r="J70" s="15"/>
+      <c r="K70" s="15"/>
+      <c r="L70" s="5"/>
+    </row>
+    <row r="71" spans="2:12">
+      <c r="B71" s="4"/>
+      <c r="C71" s="15"/>
+      <c r="D71" s="15"/>
+      <c r="E71" s="15"/>
+      <c r="F71" s="15"/>
+      <c r="G71" s="15"/>
+      <c r="H71" s="15"/>
+      <c r="I71" s="15"/>
+      <c r="J71" s="15"/>
+      <c r="K71" s="15"/>
+      <c r="L71" s="5"/>
+    </row>
+    <row r="72" spans="2:12">
+      <c r="B72" s="4"/>
+      <c r="C72" s="15"/>
+      <c r="D72" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E72" s="15"/>
+      <c r="F72" s="15"/>
+      <c r="G72" s="15"/>
+      <c r="H72" s="15"/>
+      <c r="I72" s="15"/>
+      <c r="J72" s="15"/>
+      <c r="K72" s="15"/>
+      <c r="L72" s="5"/>
+    </row>
+    <row r="73" spans="2:12">
+      <c r="B73" s="4"/>
+      <c r="C73" s="15"/>
+      <c r="D73" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E73" s="15"/>
+      <c r="F73" s="15"/>
+      <c r="G73" s="15"/>
+      <c r="H73" s="15"/>
+      <c r="I73" s="15"/>
+      <c r="J73" s="15"/>
+      <c r="K73" s="15"/>
+      <c r="L73" s="5"/>
+    </row>
+    <row r="74" spans="2:12">
+      <c r="B74" s="4"/>
+      <c r="C74" s="15"/>
+      <c r="D74" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E74" s="15"/>
+      <c r="F74" s="15"/>
+      <c r="G74" s="15"/>
+      <c r="H74" s="15"/>
+      <c r="I74" s="15"/>
+      <c r="J74" s="15"/>
+      <c r="K74" s="15"/>
+      <c r="L74" s="5"/>
+    </row>
+    <row r="75" spans="2:12">
+      <c r="B75" s="4"/>
+      <c r="C75" s="15"/>
+      <c r="D75" s="15"/>
+      <c r="E75" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F75" s="15"/>
+      <c r="G75" s="15"/>
+      <c r="H75" s="15"/>
+      <c r="I75" s="15"/>
+      <c r="J75" s="15"/>
+      <c r="K75" s="15"/>
+      <c r="L75" s="5"/>
+    </row>
+    <row r="76" spans="2:12">
+      <c r="B76" s="4"/>
+      <c r="C76" s="15"/>
+      <c r="D76" s="15"/>
+      <c r="E76" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F76" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G76" s="15"/>
+      <c r="H76" s="15"/>
+      <c r="I76" s="15"/>
+      <c r="J76" s="15"/>
+      <c r="K76" s="15"/>
+      <c r="L76" s="5"/>
+    </row>
+    <row r="77" spans="2:12">
+      <c r="B77" s="4"/>
+      <c r="C77" s="15"/>
+      <c r="D77" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E77" s="15"/>
+      <c r="F77" s="15"/>
+      <c r="G77" s="15"/>
+      <c r="H77" s="15"/>
+      <c r="I77" s="15"/>
+      <c r="J77" s="15"/>
+      <c r="K77" s="15"/>
+      <c r="L77" s="5"/>
+    </row>
+    <row r="78" spans="2:12">
+      <c r="B78" s="4"/>
+      <c r="C78" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D78" s="15"/>
+      <c r="E78" s="15"/>
+      <c r="F78" s="15"/>
+      <c r="G78" s="15"/>
+      <c r="H78" s="15"/>
+      <c r="I78" s="15"/>
+      <c r="J78" s="15"/>
+      <c r="K78" s="15"/>
+      <c r="L78" s="5"/>
+    </row>
+    <row r="79" spans="2:12">
+      <c r="B79" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C79" s="15"/>
+      <c r="D79" s="15"/>
+      <c r="E79" s="15"/>
+      <c r="F79" s="15"/>
+      <c r="G79" s="15"/>
+      <c r="H79" s="15"/>
+      <c r="I79" s="15"/>
+      <c r="J79" s="15"/>
+      <c r="K79" s="15"/>
+      <c r="L79" s="5"/>
+    </row>
+    <row r="80" spans="2:12">
+      <c r="B80" s="7"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="8"/>
+      <c r="E80" s="8"/>
+      <c r="F80" s="8"/>
+      <c r="G80" s="8"/>
+      <c r="H80" s="8"/>
+      <c r="I80" s="8"/>
+      <c r="J80" s="8"/>
+      <c r="K80" s="8"/>
+      <c r="L80" s="9"/>
+    </row>
+    <row r="113" spans="2:12">
+      <c r="B113" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C113" s="2"/>
+      <c r="D113" s="2"/>
+      <c r="E113" s="2"/>
+      <c r="F113" s="2"/>
+      <c r="G113" s="2"/>
+      <c r="H113" s="2"/>
+      <c r="I113" s="2"/>
+      <c r="J113" s="2"/>
+      <c r="K113" s="2"/>
+      <c r="L113" s="3"/>
+    </row>
+    <row r="114" spans="2:12">
+      <c r="B114" s="4"/>
+      <c r="C114" s="15"/>
+      <c r="D114" s="15"/>
+      <c r="E114" s="15"/>
+      <c r="F114" s="15"/>
+      <c r="G114" s="15"/>
+      <c r="H114" s="15"/>
+      <c r="I114" s="15"/>
+      <c r="J114" s="15"/>
+      <c r="K114" s="15"/>
+      <c r="L114" s="5"/>
+    </row>
+    <row r="115" spans="2:12">
+      <c r="B115" s="4"/>
+      <c r="C115" s="15"/>
+      <c r="D115" s="15"/>
+      <c r="E115" s="15"/>
+      <c r="F115" s="15"/>
+      <c r="G115" s="15"/>
+      <c r="H115" s="15"/>
+      <c r="I115" s="15"/>
+      <c r="J115" s="15"/>
+      <c r="K115" s="15"/>
+      <c r="L115" s="5"/>
+    </row>
+    <row r="116" spans="2:12">
+      <c r="B116" s="4"/>
+      <c r="C116" s="15"/>
+      <c r="D116" s="15"/>
+      <c r="E116" s="15"/>
+      <c r="F116" s="15"/>
+      <c r="G116" s="15"/>
+      <c r="H116" s="15"/>
+      <c r="I116" s="15"/>
+      <c r="J116" s="15"/>
+      <c r="K116" s="15"/>
+      <c r="L116" s="5"/>
+    </row>
+    <row r="117" spans="2:12">
+      <c r="B117" s="4"/>
+      <c r="C117" s="15"/>
+      <c r="D117" s="15"/>
+      <c r="E117" s="15"/>
+      <c r="F117" s="15"/>
+      <c r="G117" s="15"/>
+      <c r="H117" s="15"/>
+      <c r="I117" s="15"/>
+      <c r="J117" s="15"/>
+      <c r="K117" s="15"/>
+      <c r="L117" s="5"/>
+    </row>
+    <row r="118" spans="2:12">
+      <c r="B118" s="4"/>
+      <c r="C118" s="15"/>
+      <c r="D118" s="15"/>
+      <c r="E118" s="15"/>
+      <c r="F118" s="15"/>
+      <c r="G118" s="15"/>
+      <c r="H118" s="15"/>
+      <c r="I118" s="15"/>
+      <c r="J118" s="15"/>
+      <c r="K118" s="15"/>
+      <c r="L118" s="5"/>
+    </row>
+    <row r="119" spans="2:12">
+      <c r="B119" s="4"/>
+      <c r="C119" s="15"/>
+      <c r="D119" s="15"/>
+      <c r="E119" s="15"/>
+      <c r="F119" s="15"/>
+      <c r="G119" s="15"/>
+      <c r="H119" s="15"/>
+      <c r="I119" s="15"/>
+      <c r="J119" s="15"/>
+      <c r="K119" s="15"/>
+      <c r="L119" s="5"/>
+    </row>
+    <row r="120" spans="2:12">
+      <c r="B120" s="4"/>
+      <c r="C120" s="15"/>
+      <c r="D120" s="15"/>
+      <c r="E120" s="15"/>
+      <c r="F120" s="15"/>
+      <c r="G120" s="15"/>
+      <c r="H120" s="15"/>
+      <c r="I120" s="15"/>
+      <c r="J120" s="15"/>
+      <c r="K120" s="15"/>
+      <c r="L120" s="5"/>
+    </row>
+    <row r="121" spans="2:12">
+      <c r="B121" s="4"/>
+      <c r="C121" s="15"/>
+      <c r="D121" s="15"/>
+      <c r="E121" s="15"/>
+      <c r="F121" s="15"/>
+      <c r="G121" s="15"/>
+      <c r="H121" s="15"/>
+      <c r="I121" s="15"/>
+      <c r="J121" s="15"/>
+      <c r="K121" s="15"/>
+      <c r="L121" s="5"/>
+    </row>
+    <row r="122" spans="2:12">
+      <c r="B122" s="4"/>
+      <c r="C122" s="15"/>
+      <c r="D122" s="15"/>
+      <c r="E122" s="15"/>
+      <c r="F122" s="15"/>
+      <c r="G122" s="15"/>
+      <c r="H122" s="15"/>
+      <c r="I122" s="15"/>
+      <c r="J122" s="15"/>
+      <c r="K122" s="15"/>
+      <c r="L122" s="5"/>
+    </row>
+    <row r="123" spans="2:12">
+      <c r="B123" s="4"/>
+      <c r="C123" s="15"/>
+      <c r="D123" s="15"/>
+      <c r="E123" s="15"/>
+      <c r="F123" s="15"/>
+      <c r="G123" s="15"/>
+      <c r="H123" s="15"/>
+      <c r="I123" s="15"/>
+      <c r="J123" s="15"/>
+      <c r="K123" s="15"/>
+      <c r="L123" s="5"/>
+    </row>
+    <row r="124" spans="2:12">
+      <c r="B124" s="4"/>
+      <c r="C124" s="15"/>
+      <c r="D124" s="15"/>
+      <c r="E124" s="15"/>
+      <c r="F124" s="15"/>
+      <c r="G124" s="15"/>
+      <c r="H124" s="15"/>
+      <c r="I124" s="15"/>
+      <c r="J124" s="15"/>
+      <c r="K124" s="15"/>
+      <c r="L124" s="5"/>
+    </row>
+    <row r="125" spans="2:12">
+      <c r="B125" s="4"/>
+      <c r="C125" s="15"/>
+      <c r="D125" s="15"/>
+      <c r="E125" s="15"/>
+      <c r="F125" s="15"/>
+      <c r="G125" s="15"/>
+      <c r="H125" s="15"/>
+      <c r="I125" s="15"/>
+      <c r="J125" s="15"/>
+      <c r="K125" s="15"/>
+      <c r="L125" s="5"/>
+    </row>
+    <row r="126" spans="2:12">
+      <c r="B126" s="4"/>
+      <c r="C126" s="15"/>
+      <c r="D126" s="15"/>
+      <c r="E126" s="15"/>
+      <c r="F126" s="15"/>
+      <c r="G126" s="15"/>
+      <c r="H126" s="15"/>
+      <c r="I126" s="15"/>
+      <c r="J126" s="15"/>
+      <c r="K126" s="15"/>
+      <c r="L126" s="5"/>
+    </row>
+    <row r="127" spans="2:12">
+      <c r="B127" s="4"/>
+      <c r="C127" s="15"/>
+      <c r="D127" s="15"/>
+      <c r="E127" s="15"/>
+      <c r="F127" s="15"/>
+      <c r="G127" s="15"/>
+      <c r="H127" s="15"/>
+      <c r="I127" s="15"/>
+      <c r="J127" s="15"/>
+      <c r="K127" s="15"/>
+      <c r="L127" s="5"/>
+    </row>
+    <row r="128" spans="2:12">
+      <c r="B128" s="4"/>
+      <c r="C128" s="15"/>
+      <c r="D128" s="15"/>
+      <c r="E128" s="15"/>
+      <c r="F128" s="15"/>
+      <c r="G128" s="15"/>
+      <c r="H128" s="15"/>
+      <c r="I128" s="15"/>
+      <c r="J128" s="15"/>
+      <c r="K128" s="15"/>
+      <c r="L128" s="5"/>
+    </row>
+    <row r="129" spans="2:12">
+      <c r="B129" s="4"/>
+      <c r="C129" s="15"/>
+      <c r="D129" s="15"/>
+      <c r="E129" s="15"/>
+      <c r="F129" s="15"/>
+      <c r="G129" s="15"/>
+      <c r="H129" s="15"/>
+      <c r="I129" s="15"/>
+      <c r="J129" s="15"/>
+      <c r="K129" s="15"/>
+      <c r="L129" s="5"/>
+    </row>
+    <row r="130" spans="2:12">
+      <c r="B130" s="4"/>
+      <c r="C130" s="15"/>
+      <c r="D130" s="15"/>
+      <c r="E130" s="15"/>
+      <c r="F130" s="15"/>
+      <c r="G130" s="15"/>
+      <c r="H130" s="15"/>
+      <c r="I130" s="15"/>
+      <c r="J130" s="15"/>
+      <c r="K130" s="15"/>
+      <c r="L130" s="5"/>
+    </row>
+    <row r="131" spans="2:12">
+      <c r="B131" s="4"/>
+      <c r="C131" s="15"/>
+      <c r="D131" s="15"/>
+      <c r="E131" s="15"/>
+      <c r="F131" s="15"/>
+      <c r="G131" s="15"/>
+      <c r="H131" s="15"/>
+      <c r="I131" s="15"/>
+      <c r="J131" s="15"/>
+      <c r="K131" s="15"/>
+      <c r="L131" s="5"/>
+    </row>
+    <row r="132" spans="2:12">
+      <c r="B132" s="4"/>
+      <c r="C132" s="15"/>
+      <c r="D132" s="15"/>
+      <c r="E132" s="15"/>
+      <c r="F132" s="15"/>
+      <c r="G132" s="15"/>
+      <c r="H132" s="15"/>
+      <c r="I132" s="15"/>
+      <c r="J132" s="15"/>
+      <c r="K132" s="15"/>
+      <c r="L132" s="5"/>
+    </row>
+    <row r="133" spans="2:12">
+      <c r="B133" s="4"/>
+      <c r="C133" s="15"/>
+      <c r="D133" s="15"/>
+      <c r="E133" s="15"/>
+      <c r="F133" s="15"/>
+      <c r="G133" s="15"/>
+      <c r="H133" s="15"/>
+      <c r="I133" s="15"/>
+      <c r="J133" s="15"/>
+      <c r="K133" s="15"/>
+      <c r="L133" s="5"/>
+    </row>
+    <row r="134" spans="2:12">
+      <c r="B134" s="4"/>
+      <c r="C134" s="15"/>
+      <c r="D134" s="15"/>
+      <c r="E134" s="15"/>
+      <c r="F134" s="15"/>
+      <c r="G134" s="15"/>
+      <c r="H134" s="15"/>
+      <c r="I134" s="15"/>
+      <c r="J134" s="15"/>
+      <c r="K134" s="15"/>
+      <c r="L134" s="5"/>
+    </row>
+    <row r="135" spans="2:12">
+      <c r="B135" s="4"/>
+      <c r="C135" s="15"/>
+      <c r="D135" s="15"/>
+      <c r="E135" s="15"/>
+      <c r="F135" s="15"/>
+      <c r="G135" s="15"/>
+      <c r="H135" s="15"/>
+      <c r="I135" s="15"/>
+      <c r="J135" s="15"/>
+      <c r="K135" s="15"/>
+      <c r="L135" s="5"/>
+    </row>
+    <row r="136" spans="2:12">
+      <c r="B136" s="4"/>
+      <c r="C136" s="15"/>
+      <c r="D136" s="15"/>
+      <c r="E136" s="15"/>
+      <c r="F136" s="15"/>
+      <c r="G136" s="15"/>
+      <c r="H136" s="15"/>
+      <c r="I136" s="15"/>
+      <c r="J136" s="15"/>
+      <c r="K136" s="15"/>
+      <c r="L136" s="5"/>
+    </row>
+    <row r="137" spans="2:12">
+      <c r="B137" s="4"/>
+      <c r="C137" s="15"/>
+      <c r="D137" s="15"/>
+      <c r="E137" s="15"/>
+      <c r="F137" s="15"/>
+      <c r="G137" s="15"/>
+      <c r="H137" s="15"/>
+      <c r="I137" s="15"/>
+      <c r="J137" s="15"/>
+      <c r="K137" s="15"/>
+      <c r="L137" s="5"/>
+    </row>
+    <row r="138" spans="2:12">
+      <c r="B138" s="4"/>
+      <c r="C138" s="15"/>
+      <c r="D138" s="15"/>
+      <c r="E138" s="15"/>
+      <c r="F138" s="15"/>
+      <c r="G138" s="15"/>
+      <c r="H138" s="15"/>
+      <c r="I138" s="15"/>
+      <c r="J138" s="15"/>
+      <c r="K138" s="15"/>
+      <c r="L138" s="5"/>
+    </row>
+    <row r="139" spans="2:12">
+      <c r="B139" s="4"/>
+      <c r="C139" s="15"/>
+      <c r="D139" s="15"/>
+      <c r="E139" s="15"/>
+      <c r="F139" s="15"/>
+      <c r="G139" s="15"/>
+      <c r="H139" s="15"/>
+      <c r="I139" s="15"/>
+      <c r="J139" s="15"/>
+      <c r="K139" s="15"/>
+      <c r="L139" s="5"/>
+    </row>
+    <row r="140" spans="2:12">
+      <c r="B140" s="4"/>
+      <c r="C140" s="15"/>
+      <c r="D140" s="15"/>
+      <c r="E140" s="15"/>
+      <c r="F140" s="15"/>
+      <c r="G140" s="15"/>
+      <c r="H140" s="15"/>
+      <c r="I140" s="15"/>
+      <c r="J140" s="15"/>
+      <c r="K140" s="15"/>
+      <c r="L140" s="5"/>
+    </row>
+    <row r="141" spans="2:12">
+      <c r="B141" s="4"/>
+      <c r="C141" s="15"/>
+      <c r="D141" s="15"/>
+      <c r="E141" s="15"/>
+      <c r="F141" s="15"/>
+      <c r="G141" s="15"/>
+      <c r="H141" s="15"/>
+      <c r="I141" s="15"/>
+      <c r="J141" s="15"/>
+      <c r="K141" s="15"/>
+      <c r="L141" s="5"/>
+    </row>
+    <row r="142" spans="2:12">
+      <c r="B142" s="4"/>
+      <c r="C142" s="15"/>
+      <c r="D142" s="15"/>
+      <c r="E142" s="15"/>
+      <c r="F142" s="15"/>
+      <c r="G142" s="15"/>
+      <c r="H142" s="15"/>
+      <c r="I142" s="15"/>
+      <c r="J142" s="15"/>
+      <c r="K142" s="15"/>
+      <c r="L142" s="5"/>
+    </row>
+    <row r="143" spans="2:12">
+      <c r="B143" s="4"/>
+      <c r="C143" s="15"/>
+      <c r="D143" s="15"/>
+      <c r="E143" s="15"/>
+      <c r="F143" s="15"/>
+      <c r="G143" s="15"/>
+      <c r="H143" s="15"/>
+      <c r="I143" s="15"/>
+      <c r="J143" s="15"/>
+      <c r="K143" s="15"/>
+      <c r="L143" s="5"/>
+    </row>
+    <row r="144" spans="2:12">
+      <c r="B144" s="4"/>
+      <c r="C144" s="15"/>
+      <c r="D144" s="15"/>
+      <c r="E144" s="15"/>
+      <c r="F144" s="15"/>
+      <c r="G144" s="15"/>
+      <c r="H144" s="15"/>
+      <c r="I144" s="15"/>
+      <c r="J144" s="15"/>
+      <c r="K144" s="15"/>
+      <c r="L144" s="5"/>
+    </row>
+    <row r="145" spans="2:12">
+      <c r="B145" s="4"/>
+      <c r="C145" s="15"/>
+      <c r="D145" s="15"/>
+      <c r="E145" s="15"/>
+      <c r="F145" s="15"/>
+      <c r="G145" s="15"/>
+      <c r="H145" s="15"/>
+      <c r="I145" s="15"/>
+      <c r="J145" s="15"/>
+      <c r="K145" s="15"/>
+      <c r="L145" s="5"/>
+    </row>
+    <row r="146" spans="2:12">
+      <c r="B146" s="4"/>
+      <c r="C146" s="15"/>
+      <c r="D146" s="15"/>
+      <c r="E146" s="15"/>
+      <c r="F146" s="15"/>
+      <c r="G146" s="15"/>
+      <c r="H146" s="15"/>
+      <c r="I146" s="15"/>
+      <c r="J146" s="15"/>
+      <c r="K146" s="15"/>
+      <c r="L146" s="5"/>
+    </row>
+    <row r="147" spans="2:12">
+      <c r="B147" s="4"/>
+      <c r="C147" s="15"/>
+      <c r="D147" s="15"/>
+      <c r="E147" s="15"/>
+      <c r="F147" s="15"/>
+      <c r="G147" s="15"/>
+      <c r="H147" s="15"/>
+      <c r="I147" s="15"/>
+      <c r="J147" s="15"/>
+      <c r="K147" s="15"/>
+      <c r="L147" s="5"/>
+    </row>
+    <row r="148" spans="2:12">
+      <c r="B148" s="4"/>
+      <c r="C148" s="15"/>
+      <c r="D148" s="15"/>
+      <c r="E148" s="15"/>
+      <c r="F148" s="15"/>
+      <c r="G148" s="15"/>
+      <c r="H148" s="15"/>
+      <c r="I148" s="15"/>
+      <c r="J148" s="15"/>
+      <c r="K148" s="15"/>
+      <c r="L148" s="5"/>
+    </row>
+    <row r="149" spans="2:12">
+      <c r="B149" s="4"/>
+      <c r="C149" s="15"/>
+      <c r="D149" s="15"/>
+      <c r="E149" s="15"/>
+      <c r="F149" s="15"/>
+      <c r="G149" s="15"/>
+      <c r="H149" s="15"/>
+      <c r="I149" s="15"/>
+      <c r="J149" s="15"/>
+      <c r="K149" s="15"/>
+      <c r="L149" s="5"/>
+    </row>
+    <row r="150" spans="2:12">
+      <c r="B150" s="7"/>
+      <c r="C150" s="8"/>
+      <c r="D150" s="8"/>
+      <c r="E150" s="8"/>
+      <c r="F150" s="8"/>
+      <c r="G150" s="8"/>
+      <c r="H150" s="8"/>
+      <c r="I150" s="8"/>
+      <c r="J150" s="8"/>
+      <c r="K150" s="8"/>
+      <c r="L150" s="9"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>